<commit_message>
driver test on 11-12, camera face left and right, test in company yard and outside road, 15hz and 20hz fps.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songyang/project/code/github/vio-evaluate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38460F0-410F-724A-9CED-6A20604BC59F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA4A15A-276E-6E4D-A82F-7670E3CA8F8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12940" yWindow="920" windowWidth="27500" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="1120" windowWidth="51200" windowHeight="28340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
     <sheet name="summary" sheetId="8" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="11" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="369">
   <si>
     <t>mono+IMU</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -2310,6 +2311,18 @@
   </si>
   <si>
     <t>vel_z</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> RMSE of Pose error.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>divergent</t>
+  </si>
+  <si>
+    <t>ARW/VRW:0.66/0.11
+(Without extra noise)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2635,7 +2648,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2869,8 +2882,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -3609,6 +3628,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3741,7 +3773,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4237,13 +4269,157 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4255,139 +4431,43 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4399,75 +4479,42 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="37" fillId="34" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="37" fillId="34" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4477,17 +4524,68 @@
     <xf numFmtId="179" fontId="37" fillId="34" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="37" fillId="34" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -6229,8 +6327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38BD934-F6BF-994E-9923-4792CC496A35}">
   <dimension ref="A10:AB251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView zoomScale="131" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6293,21 +6391,21 @@
       <c r="K18" s="99"/>
     </row>
     <row r="19" spans="2:27">
-      <c r="B19" s="207" t="s">
+      <c r="B19" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="208"/>
-      <c r="D19" s="208"/>
-      <c r="E19" s="208"/>
-      <c r="F19" s="208"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
       <c r="K19" s="99"/>
-      <c r="M19" s="212" t="s">
+      <c r="M19" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="213"/>
-      <c r="O19" s="213"/>
-      <c r="P19" s="213"/>
-      <c r="Q19" s="213"/>
+      <c r="N19" s="180"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="180"/>
+      <c r="Q19" s="180"/>
     </row>
     <row r="20" spans="2:27" ht="17" thickBot="1">
       <c r="K20" s="99"/>
@@ -6323,47 +6421,47 @@
       </c>
     </row>
     <row r="21" spans="2:27">
-      <c r="B21" s="185" t="s">
+      <c r="B21" s="203" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="190"/>
-      <c r="D21" s="190" t="s">
+      <c r="C21" s="207"/>
+      <c r="D21" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="190"/>
-      <c r="F21" s="190"/>
-      <c r="G21" s="190" t="s">
+      <c r="E21" s="207"/>
+      <c r="F21" s="207"/>
+      <c r="G21" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="190"/>
-      <c r="I21" s="192"/>
+      <c r="H21" s="207"/>
+      <c r="I21" s="209"/>
       <c r="K21" s="99"/>
-      <c r="M21" s="179" t="s">
+      <c r="M21" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="N21" s="181"/>
-      <c r="O21" s="181" t="s">
+      <c r="N21" s="176"/>
+      <c r="O21" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="P21" s="181"/>
-      <c r="Q21" s="181"/>
-      <c r="R21" s="181" t="s">
+      <c r="P21" s="176"/>
+      <c r="Q21" s="176"/>
+      <c r="R21" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="S21" s="181"/>
-      <c r="T21" s="209"/>
-      <c r="V21" s="179" t="s">
+      <c r="S21" s="176"/>
+      <c r="T21" s="177"/>
+      <c r="V21" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="W21" s="181"/>
-      <c r="X21" s="204" t="s">
+      <c r="W21" s="176"/>
+      <c r="X21" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="Y21" s="205"/>
+      <c r="Y21" s="189"/>
     </row>
     <row r="22" spans="2:27">
-      <c r="B22" s="166"/>
-      <c r="C22" s="191"/>
+      <c r="B22" s="192"/>
+      <c r="C22" s="208"/>
       <c r="D22" s="14" t="s">
         <v>7</v>
       </c>
@@ -6383,8 +6481,8 @@
         <v>2</v>
       </c>
       <c r="K22" s="99"/>
-      <c r="M22" s="180"/>
-      <c r="N22" s="182"/>
+      <c r="M22" s="182"/>
+      <c r="N22" s="183"/>
       <c r="O22" s="69" t="s">
         <v>7</v>
       </c>
@@ -6403,8 +6501,8 @@
       <c r="T22" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="V22" s="180"/>
-      <c r="W22" s="182"/>
+      <c r="V22" s="182"/>
+      <c r="W22" s="183"/>
       <c r="X22" s="114" t="s">
         <v>316</v>
       </c>
@@ -6413,7 +6511,7 @@
       </c>
     </row>
     <row r="23" spans="2:27">
-      <c r="B23" s="166" t="s">
+      <c r="B23" s="192" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -6425,16 +6523,16 @@
       <c r="E23" s="4">
         <v>0.27986669502740003</v>
       </c>
-      <c r="F23" s="193"/>
+      <c r="F23" s="194"/>
       <c r="G23" s="4">
         <v>0.68010270563139996</v>
       </c>
       <c r="H23" s="4">
         <v>0.66187876247435995</v>
       </c>
-      <c r="I23" s="194"/>
+      <c r="I23" s="173"/>
       <c r="K23" s="99"/>
-      <c r="M23" s="177" t="s">
+      <c r="M23" s="170" t="s">
         <v>11</v>
       </c>
       <c r="N23" s="63" t="s">
@@ -6446,15 +6544,15 @@
       <c r="P23" s="64">
         <v>0.28282051441461498</v>
       </c>
-      <c r="Q23" s="215"/>
+      <c r="Q23" s="171"/>
       <c r="R23" s="64">
         <v>0.62156490272548404</v>
       </c>
       <c r="S23" s="64">
         <v>0.58449899330501398</v>
       </c>
-      <c r="T23" s="210"/>
-      <c r="V23" s="177" t="s">
+      <c r="T23" s="168"/>
+      <c r="V23" s="170" t="s">
         <v>10</v>
       </c>
       <c r="W23" s="63" t="s">
@@ -6463,13 +6561,13 @@
       <c r="X23" s="64">
         <v>8.2978075999999998E-2</v>
       </c>
-      <c r="Y23" s="215"/>
-      <c r="AA23" s="200" t="s">
+      <c r="Y23" s="171"/>
+      <c r="AA23" s="169" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:27">
-      <c r="B24" s="166"/>
+      <c r="B24" s="192"/>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -6479,16 +6577,16 @@
       <c r="E24" s="4">
         <v>0.31159143254010802</v>
       </c>
-      <c r="F24" s="193"/>
+      <c r="F24" s="194"/>
       <c r="G24" s="4">
         <v>0.52286421194715804</v>
       </c>
       <c r="H24" s="4">
         <v>0.53292639849711798</v>
       </c>
-      <c r="I24" s="194"/>
+      <c r="I24" s="173"/>
       <c r="K24" s="99"/>
-      <c r="M24" s="177"/>
+      <c r="M24" s="170"/>
       <c r="N24" s="63" t="s">
         <v>6</v>
       </c>
@@ -6498,26 +6596,26 @@
       <c r="P24" s="64">
         <v>0.24132286832387601</v>
       </c>
-      <c r="Q24" s="215"/>
+      <c r="Q24" s="171"/>
       <c r="R24" s="64">
         <v>0.45448695005226902</v>
       </c>
       <c r="S24" s="64">
         <v>0.44134917356160802</v>
       </c>
-      <c r="T24" s="210"/>
-      <c r="V24" s="177"/>
+      <c r="T24" s="168"/>
+      <c r="V24" s="170"/>
       <c r="W24" s="63" t="s">
         <v>6</v>
       </c>
       <c r="X24" s="64">
         <v>9.9679073000000007E-2</v>
       </c>
-      <c r="Y24" s="215"/>
-      <c r="AA24" s="200"/>
+      <c r="Y24" s="171"/>
+      <c r="AA24" s="169"/>
     </row>
     <row r="25" spans="2:27">
-      <c r="B25" s="166"/>
+      <c r="B25" s="192"/>
       <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
@@ -6527,16 +6625,16 @@
       <c r="E25" s="4">
         <v>0.25367114103762001</v>
       </c>
-      <c r="F25" s="193"/>
+      <c r="F25" s="194"/>
       <c r="G25" s="4">
         <v>0.15005929600283599</v>
       </c>
       <c r="H25" s="4">
         <v>2.1150037658527399E-2</v>
       </c>
-      <c r="I25" s="194"/>
+      <c r="I25" s="173"/>
       <c r="K25" s="99"/>
-      <c r="M25" s="177"/>
+      <c r="M25" s="170"/>
       <c r="N25" s="63" t="s">
         <v>5</v>
       </c>
@@ -6546,26 +6644,26 @@
       <c r="P25" s="64">
         <v>0.17953083576787501</v>
       </c>
-      <c r="Q25" s="215"/>
+      <c r="Q25" s="171"/>
       <c r="R25" s="64">
         <v>0.26264407173694898</v>
       </c>
       <c r="S25" s="64">
         <v>0.164907276430004</v>
       </c>
-      <c r="T25" s="210"/>
-      <c r="V25" s="177"/>
+      <c r="T25" s="168"/>
+      <c r="V25" s="170"/>
       <c r="W25" s="63" t="s">
         <v>5</v>
       </c>
       <c r="X25" s="64">
         <v>2.9346153E-2</v>
       </c>
-      <c r="Y25" s="215"/>
-      <c r="AA25" s="200"/>
+      <c r="Y25" s="171"/>
+      <c r="AA25" s="169"/>
     </row>
     <row r="26" spans="2:27">
-      <c r="B26" s="166"/>
+      <c r="B26" s="192"/>
       <c r="C26" s="3" t="s">
         <v>4</v>
       </c>
@@ -6588,7 +6686,7 @@
         <v>0.1</v>
       </c>
       <c r="K26" s="99"/>
-      <c r="M26" s="177"/>
+      <c r="M26" s="170"/>
       <c r="N26" s="63" t="s">
         <v>4</v>
       </c>
@@ -6610,7 +6708,7 @@
       <c r="T26" s="73">
         <v>0.1</v>
       </c>
-      <c r="V26" s="177"/>
+      <c r="V26" s="170"/>
       <c r="W26" s="63" t="s">
         <v>4</v>
       </c>
@@ -6620,10 +6718,10 @@
       <c r="Y26" s="72">
         <v>0.09</v>
       </c>
-      <c r="AA26" s="200"/>
+      <c r="AA26" s="169"/>
     </row>
     <row r="27" spans="2:27">
-      <c r="B27" s="166" t="s">
+      <c r="B27" s="192" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -6635,16 +6733,16 @@
       <c r="E27" s="4">
         <v>2.2822992480011099</v>
       </c>
-      <c r="F27" s="193"/>
+      <c r="F27" s="194"/>
       <c r="G27" s="4">
         <v>2.0418759425309498</v>
       </c>
       <c r="H27" s="4">
         <v>2.0473786537993699</v>
       </c>
-      <c r="I27" s="194"/>
+      <c r="I27" s="173"/>
       <c r="K27" s="99"/>
-      <c r="M27" s="200" t="s">
+      <c r="M27" s="169" t="s">
         <v>10</v>
       </c>
       <c r="N27" s="65" t="s">
@@ -6656,15 +6754,15 @@
       <c r="P27" s="66">
         <v>0.13413593611147401</v>
       </c>
-      <c r="Q27" s="214"/>
+      <c r="Q27" s="172"/>
       <c r="R27" s="66">
         <v>0.30682580514694002</v>
       </c>
       <c r="S27" s="66">
         <v>0.31669906694920302</v>
       </c>
-      <c r="T27" s="211"/>
-      <c r="V27" s="200" t="s">
+      <c r="T27" s="178"/>
+      <c r="V27" s="169" t="s">
         <v>11</v>
       </c>
       <c r="W27" s="65" t="s">
@@ -6673,10 +6771,10 @@
       <c r="X27" s="66">
         <v>8.6425494000000005E-2</v>
       </c>
-      <c r="Y27" s="214"/>
+      <c r="Y27" s="172"/>
     </row>
     <row r="28" spans="2:27">
-      <c r="B28" s="166"/>
+      <c r="B28" s="192"/>
       <c r="C28" s="4" t="s">
         <v>6</v>
       </c>
@@ -6686,16 +6784,16 @@
       <c r="E28" s="4">
         <v>2.1380731358266098</v>
       </c>
-      <c r="F28" s="193"/>
+      <c r="F28" s="194"/>
       <c r="G28" s="4">
         <v>2.12584725653074</v>
       </c>
       <c r="H28" s="4">
         <v>2.2110485659725998</v>
       </c>
-      <c r="I28" s="194"/>
+      <c r="I28" s="173"/>
       <c r="K28" s="99"/>
-      <c r="M28" s="200"/>
+      <c r="M28" s="169"/>
       <c r="N28" s="65" t="s">
         <v>6</v>
       </c>
@@ -6705,25 +6803,25 @@
       <c r="P28" s="66">
         <v>0.103259079645247</v>
       </c>
-      <c r="Q28" s="214"/>
+      <c r="Q28" s="172"/>
       <c r="R28" s="66">
         <v>0.106026794417206</v>
       </c>
       <c r="S28" s="66">
         <v>8.0984201915277998E-2</v>
       </c>
-      <c r="T28" s="211"/>
-      <c r="V28" s="200"/>
+      <c r="T28" s="178"/>
+      <c r="V28" s="169"/>
       <c r="W28" s="65" t="s">
         <v>6</v>
       </c>
       <c r="X28" s="66">
         <v>0.109670028</v>
       </c>
-      <c r="Y28" s="214"/>
+      <c r="Y28" s="172"/>
     </row>
     <row r="29" spans="2:27">
-      <c r="B29" s="166"/>
+      <c r="B29" s="192"/>
       <c r="C29" s="4" t="s">
         <v>5</v>
       </c>
@@ -6733,16 +6831,16 @@
       <c r="E29" s="4">
         <v>1.25058960412151E-2</v>
       </c>
-      <c r="F29" s="193"/>
+      <c r="F29" s="194"/>
       <c r="G29" s="4">
         <v>0.178954364917943</v>
       </c>
       <c r="H29" s="4">
         <v>6.4240433002411002E-2</v>
       </c>
-      <c r="I29" s="194"/>
+      <c r="I29" s="173"/>
       <c r="K29" s="99"/>
-      <c r="M29" s="200"/>
+      <c r="M29" s="169"/>
       <c r="N29" s="65" t="s">
         <v>5</v>
       </c>
@@ -6752,25 +6850,25 @@
       <c r="P29" s="66">
         <v>2.2541432670424199E-2</v>
       </c>
-      <c r="Q29" s="214"/>
+      <c r="Q29" s="172"/>
       <c r="R29" s="66">
         <v>0.20115670057829299</v>
       </c>
       <c r="S29" s="66">
         <v>8.8748332176745603E-2</v>
       </c>
-      <c r="T29" s="211"/>
-      <c r="V29" s="200"/>
+      <c r="T29" s="178"/>
+      <c r="V29" s="169"/>
       <c r="W29" s="65" t="s">
         <v>5</v>
       </c>
       <c r="X29" s="66">
         <v>0.16404260400000001</v>
       </c>
-      <c r="Y29" s="214"/>
+      <c r="Y29" s="172"/>
     </row>
     <row r="30" spans="2:27">
-      <c r="B30" s="166"/>
+      <c r="B30" s="192"/>
       <c r="C30" s="4" t="s">
         <v>4</v>
       </c>
@@ -6793,7 +6891,7 @@
         <v>0.18</v>
       </c>
       <c r="K30" s="99"/>
-      <c r="M30" s="200"/>
+      <c r="M30" s="169"/>
       <c r="N30" s="65" t="s">
         <v>4</v>
       </c>
@@ -6815,7 +6913,7 @@
       <c r="T30" s="76">
         <v>0.18</v>
       </c>
-      <c r="V30" s="200"/>
+      <c r="V30" s="169"/>
       <c r="W30" s="65" t="s">
         <v>4</v>
       </c>
@@ -6827,7 +6925,7 @@
       </c>
     </row>
     <row r="31" spans="2:27">
-      <c r="B31" s="166" t="s">
+      <c r="B31" s="192" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -6839,16 +6937,16 @@
       <c r="E31" s="6">
         <v>0.27090614469824897</v>
       </c>
-      <c r="F31" s="193"/>
+      <c r="F31" s="194"/>
       <c r="G31" s="6">
         <v>0.374535506890527</v>
       </c>
       <c r="H31" s="6">
         <v>0.24745172364194501</v>
       </c>
-      <c r="I31" s="194"/>
+      <c r="I31" s="173"/>
       <c r="K31" s="99"/>
-      <c r="M31" s="177" t="s">
+      <c r="M31" s="170" t="s">
         <v>12</v>
       </c>
       <c r="N31" s="67" t="s">
@@ -6860,15 +6958,15 @@
       <c r="P31" s="64">
         <v>0.39845133051777398</v>
       </c>
-      <c r="Q31" s="206"/>
+      <c r="Q31" s="190"/>
       <c r="R31" s="64">
         <v>0.34457062215270401</v>
       </c>
       <c r="S31" s="64">
         <v>0.19777353314753901</v>
       </c>
-      <c r="T31" s="210"/>
-      <c r="V31" s="177" t="s">
+      <c r="T31" s="168"/>
+      <c r="V31" s="170" t="s">
         <v>12</v>
       </c>
       <c r="W31" s="67" t="s">
@@ -6877,10 +6975,10 @@
       <c r="X31" s="64">
         <v>0.190903462</v>
       </c>
-      <c r="Y31" s="206"/>
+      <c r="Y31" s="190"/>
     </row>
     <row r="32" spans="2:27">
-      <c r="B32" s="166"/>
+      <c r="B32" s="192"/>
       <c r="C32" s="4" t="s">
         <v>6</v>
       </c>
@@ -6890,16 +6988,16 @@
       <c r="E32" s="6">
         <v>0.36111271508034998</v>
       </c>
-      <c r="F32" s="193"/>
+      <c r="F32" s="194"/>
       <c r="G32" s="6">
         <v>0.58021180541887096</v>
       </c>
       <c r="H32" s="6">
         <v>0.31234903625947402</v>
       </c>
-      <c r="I32" s="194"/>
+      <c r="I32" s="173"/>
       <c r="K32" s="99"/>
-      <c r="M32" s="177"/>
+      <c r="M32" s="170"/>
       <c r="N32" s="67" t="s">
         <v>6</v>
       </c>
@@ -6909,25 +7007,25 @@
       <c r="P32" s="64">
         <v>0.57775878419396398</v>
       </c>
-      <c r="Q32" s="206"/>
+      <c r="Q32" s="190"/>
       <c r="R32" s="64">
         <v>0.36014131193795101</v>
       </c>
       <c r="S32" s="64">
         <v>0.166267990931902</v>
       </c>
-      <c r="T32" s="210"/>
-      <c r="V32" s="177"/>
+      <c r="T32" s="168"/>
+      <c r="V32" s="170"/>
       <c r="W32" s="67" t="s">
         <v>6</v>
       </c>
       <c r="X32" s="64">
         <v>0.26741922000000001</v>
       </c>
-      <c r="Y32" s="206"/>
+      <c r="Y32" s="190"/>
     </row>
     <row r="33" spans="2:26">
-      <c r="B33" s="166"/>
+      <c r="B33" s="192"/>
       <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
@@ -6937,16 +7035,16 @@
       <c r="E33" s="6">
         <v>6.4442896226864096E-2</v>
       </c>
-      <c r="F33" s="193"/>
+      <c r="F33" s="194"/>
       <c r="G33" s="6">
         <v>6.60773004717118E-2</v>
       </c>
       <c r="H33" s="6">
         <v>4.60370898663078E-2</v>
       </c>
-      <c r="I33" s="194"/>
+      <c r="I33" s="173"/>
       <c r="K33" s="99"/>
-      <c r="M33" s="177"/>
+      <c r="M33" s="170"/>
       <c r="N33" s="67" t="s">
         <v>5</v>
       </c>
@@ -6956,25 +7054,25 @@
       <c r="P33" s="64">
         <v>0.11818657724488101</v>
       </c>
-      <c r="Q33" s="206"/>
+      <c r="Q33" s="190"/>
       <c r="R33" s="64">
         <v>0.269305774789453</v>
       </c>
       <c r="S33" s="64">
         <v>0.274170392820758</v>
       </c>
-      <c r="T33" s="210"/>
-      <c r="V33" s="177"/>
+      <c r="T33" s="168"/>
+      <c r="V33" s="170"/>
       <c r="W33" s="67" t="s">
         <v>5</v>
       </c>
       <c r="X33" s="64">
         <v>0.17281497700000001</v>
       </c>
-      <c r="Y33" s="206"/>
+      <c r="Y33" s="190"/>
     </row>
     <row r="34" spans="2:26" ht="17" thickBot="1">
-      <c r="B34" s="167"/>
+      <c r="B34" s="193"/>
       <c r="C34" s="10" t="s">
         <v>4</v>
       </c>
@@ -6997,7 +7095,7 @@
         <v>0.27</v>
       </c>
       <c r="K34" s="99"/>
-      <c r="M34" s="178"/>
+      <c r="M34" s="187"/>
       <c r="N34" s="68" t="s">
         <v>4</v>
       </c>
@@ -7019,7 +7117,7 @@
       <c r="T34" s="79">
         <v>0.27</v>
       </c>
-      <c r="V34" s="178"/>
+      <c r="V34" s="187"/>
       <c r="W34" s="68" t="s">
         <v>4</v>
       </c>
@@ -7043,42 +7141,42 @@
       <c r="K38" s="99"/>
     </row>
     <row r="39" spans="2:26">
-      <c r="B39" s="185" t="s">
+      <c r="B39" s="203" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="198"/>
-      <c r="D39" s="165" t="s">
+      <c r="C39" s="201"/>
+      <c r="D39" s="198" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
-      <c r="H39" s="197"/>
+      <c r="E39" s="199"/>
+      <c r="F39" s="199"/>
+      <c r="G39" s="199"/>
+      <c r="H39" s="200"/>
       <c r="K39" s="99"/>
-      <c r="M39" s="179" t="s">
+      <c r="M39" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="N39" s="181"/>
-      <c r="O39" s="202" t="s">
+      <c r="N39" s="176"/>
+      <c r="O39" s="185" t="s">
         <v>46</v>
       </c>
-      <c r="P39" s="202"/>
-      <c r="Q39" s="202"/>
-      <c r="R39" s="202"/>
-      <c r="S39" s="203"/>
-      <c r="V39" s="179" t="s">
+      <c r="P39" s="185"/>
+      <c r="Q39" s="185"/>
+      <c r="R39" s="185"/>
+      <c r="S39" s="186"/>
+      <c r="V39" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="W39" s="181"/>
-      <c r="X39" s="202" t="s">
+      <c r="W39" s="176"/>
+      <c r="X39" s="185" t="s">
         <v>254</v>
       </c>
-      <c r="Y39" s="202"/>
-      <c r="Z39" s="203"/>
+      <c r="Y39" s="185"/>
+      <c r="Z39" s="186"/>
     </row>
     <row r="40" spans="2:26" ht="42" customHeight="1" thickBot="1">
-      <c r="B40" s="184"/>
-      <c r="C40" s="199"/>
+      <c r="B40" s="204"/>
+      <c r="C40" s="202"/>
       <c r="D40" s="40" t="s">
         <v>14</v>
       </c>
@@ -7095,8 +7193,8 @@
         <v>39</v>
       </c>
       <c r="K40" s="99"/>
-      <c r="M40" s="180"/>
-      <c r="N40" s="182"/>
+      <c r="M40" s="182"/>
+      <c r="N40" s="183"/>
       <c r="O40" s="88" t="s">
         <v>252</v>
       </c>
@@ -7112,8 +7210,8 @@
       <c r="S40" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="V40" s="180"/>
-      <c r="W40" s="182"/>
+      <c r="V40" s="182"/>
+      <c r="W40" s="183"/>
       <c r="X40" s="88" t="s">
         <v>253</v>
       </c>
@@ -7125,7 +7223,7 @@
       </c>
     </row>
     <row r="41" spans="2:26">
-      <c r="B41" s="185" t="s">
+      <c r="B41" s="203" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -7147,7 +7245,7 @@
         <v>0.28327658999999999</v>
       </c>
       <c r="K41" s="99"/>
-      <c r="M41" s="177" t="s">
+      <c r="M41" s="170" t="s">
         <v>11</v>
       </c>
       <c r="N41" s="80" t="s">
@@ -7168,7 +7266,7 @@
       <c r="S41" s="81">
         <v>0.28327658999999999</v>
       </c>
-      <c r="V41" s="177" t="s">
+      <c r="V41" s="170" t="s">
         <v>11</v>
       </c>
       <c r="W41" s="80" t="s">
@@ -7185,7 +7283,7 @@
       </c>
     </row>
     <row r="42" spans="2:26">
-      <c r="B42" s="166"/>
+      <c r="B42" s="192"/>
       <c r="C42" s="14" t="s">
         <v>54</v>
       </c>
@@ -7205,7 +7303,7 @@
         <v>0.39291767999999999</v>
       </c>
       <c r="K42" s="99"/>
-      <c r="M42" s="177"/>
+      <c r="M42" s="170"/>
       <c r="N42" s="80" t="s">
         <v>54</v>
       </c>
@@ -7224,7 +7322,7 @@
       <c r="S42" s="81">
         <v>0.39291767999999999</v>
       </c>
-      <c r="V42" s="177"/>
+      <c r="V42" s="170"/>
       <c r="W42" s="80" t="s">
         <v>54</v>
       </c>
@@ -7239,7 +7337,7 @@
       </c>
     </row>
     <row r="43" spans="2:26">
-      <c r="B43" s="166"/>
+      <c r="B43" s="192"/>
       <c r="C43" s="14" t="s">
         <v>55</v>
       </c>
@@ -7259,7 +7357,7 @@
         <v>0.28943322799999999</v>
       </c>
       <c r="K43" s="99"/>
-      <c r="M43" s="177"/>
+      <c r="M43" s="170"/>
       <c r="N43" s="80" t="s">
         <v>55</v>
       </c>
@@ -7278,7 +7376,7 @@
       <c r="S43" s="81">
         <v>0.28943322799999999</v>
       </c>
-      <c r="V43" s="177"/>
+      <c r="V43" s="170"/>
       <c r="W43" s="80" t="s">
         <v>55</v>
       </c>
@@ -7293,7 +7391,7 @@
       </c>
     </row>
     <row r="44" spans="2:26" ht="17" thickBot="1">
-      <c r="B44" s="167"/>
+      <c r="B44" s="193"/>
       <c r="C44" s="37" t="s">
         <v>56</v>
       </c>
@@ -7313,7 +7411,7 @@
         <v>0.56702118099999999</v>
       </c>
       <c r="K44" s="99"/>
-      <c r="M44" s="177"/>
+      <c r="M44" s="170"/>
       <c r="N44" s="80" t="s">
         <v>56</v>
       </c>
@@ -7332,7 +7430,7 @@
       <c r="S44" s="85">
         <v>0.56702118099999999</v>
       </c>
-      <c r="V44" s="178"/>
+      <c r="V44" s="187"/>
       <c r="W44" s="89" t="s">
         <v>56</v>
       </c>
@@ -7347,7 +7445,7 @@
       </c>
     </row>
     <row r="45" spans="2:26" ht="16" customHeight="1">
-      <c r="B45" s="183" t="s">
+      <c r="B45" s="191" t="s">
         <v>10</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -7369,7 +7467,7 @@
         <v>2.2233044049999999</v>
       </c>
       <c r="K45" s="99"/>
-      <c r="M45" s="200" t="s">
+      <c r="M45" s="169" t="s">
         <v>10</v>
       </c>
       <c r="N45" s="82" t="s">
@@ -7392,7 +7490,7 @@
       </c>
     </row>
     <row r="46" spans="2:26">
-      <c r="B46" s="166"/>
+      <c r="B46" s="192"/>
       <c r="C46" s="14" t="s">
         <v>54</v>
       </c>
@@ -7412,7 +7510,7 @@
         <v>2.0428535559999998</v>
       </c>
       <c r="K46" s="99"/>
-      <c r="M46" s="200"/>
+      <c r="M46" s="169"/>
       <c r="N46" s="82" t="s">
         <v>54</v>
       </c>
@@ -7433,7 +7531,7 @@
       </c>
     </row>
     <row r="47" spans="2:26">
-      <c r="B47" s="166"/>
+      <c r="B47" s="192"/>
       <c r="C47" s="14" t="s">
         <v>55</v>
       </c>
@@ -7453,7 +7551,7 @@
         <v>1.4747674000000001E-2</v>
       </c>
       <c r="K47" s="99"/>
-      <c r="M47" s="200"/>
+      <c r="M47" s="169"/>
       <c r="N47" s="82" t="s">
         <v>55</v>
       </c>
@@ -7474,7 +7572,7 @@
       </c>
     </row>
     <row r="48" spans="2:26" ht="17" thickBot="1">
-      <c r="B48" s="167"/>
+      <c r="B48" s="193"/>
       <c r="C48" s="37" t="s">
         <v>56</v>
       </c>
@@ -7494,7 +7592,7 @@
         <v>3.0193695030000001</v>
       </c>
       <c r="K48" s="99"/>
-      <c r="M48" s="201"/>
+      <c r="M48" s="184"/>
       <c r="N48" s="84" t="s">
         <v>56</v>
       </c>
@@ -7516,16 +7614,16 @@
     </row>
     <row r="49" spans="2:28" ht="17" customHeight="1" thickBot="1">
       <c r="K49" s="99"/>
-      <c r="V49" s="179" t="s">
+      <c r="V49" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="W49" s="181"/>
-      <c r="X49" s="174" t="s">
+      <c r="W49" s="176"/>
+      <c r="X49" s="210" t="s">
         <v>257</v>
       </c>
-      <c r="Y49" s="175"/>
-      <c r="Z49" s="175"/>
-      <c r="AA49" s="176"/>
+      <c r="Y49" s="211"/>
+      <c r="Z49" s="211"/>
+      <c r="AA49" s="212"/>
     </row>
     <row r="50" spans="2:28" ht="53">
       <c r="F50" s="16" t="s">
@@ -7536,8 +7634,8 @@
       </c>
       <c r="H50" s="50"/>
       <c r="K50" s="99"/>
-      <c r="V50" s="180"/>
-      <c r="W50" s="182"/>
+      <c r="V50" s="182"/>
+      <c r="W50" s="183"/>
       <c r="X50" s="88" t="s">
         <v>253</v>
       </c>
@@ -7555,14 +7653,14 @@
       <c r="F51" s="2">
         <v>0.39651994499999998</v>
       </c>
-      <c r="G51" s="195" t="s">
+      <c r="G51" s="197" t="s">
         <v>59</v>
       </c>
-      <c r="H51" s="188" t="s">
+      <c r="H51" s="205" t="s">
         <v>60</v>
       </c>
       <c r="K51" s="99"/>
-      <c r="V51" s="177" t="s">
+      <c r="V51" s="170" t="s">
         <v>11</v>
       </c>
       <c r="W51" s="80" t="s">
@@ -7585,10 +7683,10 @@
       <c r="F52" s="2">
         <v>0.43426528800000003</v>
       </c>
-      <c r="G52" s="195"/>
-      <c r="H52" s="188"/>
+      <c r="G52" s="197"/>
+      <c r="H52" s="205"/>
       <c r="K52" s="99"/>
-      <c r="V52" s="177"/>
+      <c r="V52" s="170"/>
       <c r="W52" s="80" t="s">
         <v>54</v>
       </c>
@@ -7609,10 +7707,10 @@
       <c r="F53" s="2">
         <v>0.20012048199999999</v>
       </c>
-      <c r="G53" s="195"/>
-      <c r="H53" s="188"/>
+      <c r="G53" s="197"/>
+      <c r="H53" s="205"/>
       <c r="K53" s="99"/>
-      <c r="V53" s="177"/>
+      <c r="V53" s="170"/>
       <c r="W53" s="80" t="s">
         <v>55</v>
       </c>
@@ -7633,10 +7731,10 @@
       <c r="F54" s="2">
         <v>0.63796581399999996</v>
       </c>
-      <c r="G54" s="195"/>
-      <c r="H54" s="189"/>
+      <c r="G54" s="197"/>
+      <c r="H54" s="206"/>
       <c r="K54" s="99"/>
-      <c r="V54" s="178"/>
+      <c r="V54" s="187"/>
       <c r="W54" s="89" t="s">
         <v>56</v>
       </c>
@@ -7732,7 +7830,7 @@
       </c>
     </row>
     <row r="58" spans="2:28" ht="16" customHeight="1">
-      <c r="B58" s="186" t="s">
+      <c r="B58" s="195" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="20" t="s">
@@ -7758,7 +7856,7 @@
         <v>2.2240023253263277</v>
       </c>
       <c r="K58" s="99"/>
-      <c r="M58" s="186" t="s">
+      <c r="M58" s="195" t="s">
         <v>15</v>
       </c>
       <c r="N58" s="58" t="s">
@@ -7783,7 +7881,7 @@
         <f>AVERAGE(O58:S58)</f>
         <v>0.14872877913523658</v>
       </c>
-      <c r="V58" s="177" t="s">
+      <c r="V58" s="170" t="s">
         <v>11</v>
       </c>
       <c r="W58" s="96" t="s">
@@ -7806,7 +7904,7 @@
       </c>
     </row>
     <row r="59" spans="2:28">
-      <c r="B59" s="186"/>
+      <c r="B59" s="195"/>
       <c r="C59" s="2" t="s">
         <v>17</v>
       </c>
@@ -7830,7 +7928,7 @@
         <v>2.0431343345966879</v>
       </c>
       <c r="K59" s="99"/>
-      <c r="M59" s="186"/>
+      <c r="M59" s="195"/>
       <c r="N59" s="56" t="s">
         <v>17</v>
       </c>
@@ -7853,7 +7951,7 @@
         <f>AVERAGE(O59:S59)</f>
         <v>0.14057854177558421</v>
       </c>
-      <c r="V59" s="177"/>
+      <c r="V59" s="170"/>
       <c r="W59" s="97" t="s">
         <v>17</v>
       </c>
@@ -7874,7 +7972,7 @@
       </c>
     </row>
     <row r="60" spans="2:28">
-      <c r="B60" s="186"/>
+      <c r="B60" s="195"/>
       <c r="C60" s="2" t="s">
         <v>18</v>
       </c>
@@ -7899,7 +7997,7 @@
       </c>
       <c r="K60" s="99"/>
       <c r="L60" s="25"/>
-      <c r="M60" s="186"/>
+      <c r="M60" s="195"/>
       <c r="N60" s="56" t="s">
         <v>18</v>
       </c>
@@ -7922,7 +8020,7 @@
         <f>AVERAGE(O60:S60)</f>
         <v>2.9979485376045799E-2</v>
       </c>
-      <c r="V60" s="177"/>
+      <c r="V60" s="170"/>
       <c r="W60" s="97" t="s">
         <v>18</v>
       </c>
@@ -7943,7 +8041,7 @@
       </c>
     </row>
     <row r="61" spans="2:28" ht="17" thickBot="1">
-      <c r="B61" s="187"/>
+      <c r="B61" s="196"/>
       <c r="C61" s="18" t="s">
         <v>19</v>
       </c>
@@ -7967,7 +8065,7 @@
         <v>3.0200654405003959</v>
       </c>
       <c r="K61" s="99"/>
-      <c r="M61" s="187"/>
+      <c r="M61" s="196"/>
       <c r="N61" s="59" t="s">
         <v>19</v>
       </c>
@@ -7990,7 +8088,7 @@
         <f>AVERAGE(O61:S61)</f>
         <v>0.20685651882384262</v>
       </c>
-      <c r="V61" s="178"/>
+      <c r="V61" s="187"/>
       <c r="W61" s="98" t="s">
         <v>19</v>
       </c>
@@ -8054,7 +8152,7 @@
       </c>
     </row>
     <row r="63" spans="2:28">
-      <c r="B63" s="186" t="s">
+      <c r="B63" s="195" t="s">
         <v>36</v>
       </c>
       <c r="C63" s="20" t="s">
@@ -8080,7 +8178,7 @@
         <v>2.2242837265980882</v>
       </c>
       <c r="K63" s="99"/>
-      <c r="M63" s="186" t="s">
+      <c r="M63" s="195" t="s">
         <v>36</v>
       </c>
       <c r="N63" s="20" t="s">
@@ -8107,7 +8205,7 @@
       </c>
     </row>
     <row r="64" spans="2:28">
-      <c r="B64" s="186"/>
+      <c r="B64" s="195"/>
       <c r="C64" s="2" t="s">
         <v>17</v>
       </c>
@@ -8131,7 +8229,7 @@
         <v>2.0441570856025177</v>
       </c>
       <c r="K64" s="99"/>
-      <c r="M64" s="186"/>
+      <c r="M64" s="195"/>
       <c r="N64" s="2" t="s">
         <v>17</v>
       </c>
@@ -8156,7 +8254,7 @@
       </c>
     </row>
     <row r="65" spans="2:28">
-      <c r="B65" s="186"/>
+      <c r="B65" s="195"/>
       <c r="C65" s="2" t="s">
         <v>18</v>
       </c>
@@ -8181,7 +8279,7 @@
       </c>
       <c r="K65" s="99"/>
       <c r="L65" s="25"/>
-      <c r="M65" s="186"/>
+      <c r="M65" s="195"/>
       <c r="N65" s="2" t="s">
         <v>18</v>
       </c>
@@ -8206,7 +8304,7 @@
       </c>
     </row>
     <row r="66" spans="2:28" ht="17" thickBot="1">
-      <c r="B66" s="187"/>
+      <c r="B66" s="196"/>
       <c r="C66" s="18" t="s">
         <v>19</v>
       </c>
@@ -8230,7 +8328,7 @@
         <v>3.0209650878054681</v>
       </c>
       <c r="K66" s="99"/>
-      <c r="M66" s="187"/>
+      <c r="M66" s="196"/>
       <c r="N66" s="18" t="s">
         <v>19</v>
       </c>
@@ -8298,7 +8396,7 @@
       </c>
     </row>
     <row r="68" spans="2:28">
-      <c r="B68" s="186" t="s">
+      <c r="B68" s="195" t="s">
         <v>38</v>
       </c>
       <c r="C68" s="20" t="s">
@@ -8324,7 +8422,7 @@
         <v>2.2282666299559977</v>
       </c>
       <c r="K68" s="99"/>
-      <c r="M68" s="186" t="s">
+      <c r="M68" s="195" t="s">
         <v>38</v>
       </c>
       <c r="N68" s="20" t="s">
@@ -8372,7 +8470,7 @@
       </c>
     </row>
     <row r="69" spans="2:28" ht="34">
-      <c r="B69" s="186"/>
+      <c r="B69" s="195"/>
       <c r="C69" s="2" t="s">
         <v>17</v>
       </c>
@@ -8396,7 +8494,7 @@
         <v>2.0439806658106678</v>
       </c>
       <c r="K69" s="99"/>
-      <c r="M69" s="186"/>
+      <c r="M69" s="195"/>
       <c r="N69" s="2" t="s">
         <v>17</v>
       </c>
@@ -8442,7 +8540,7 @@
       </c>
     </row>
     <row r="70" spans="2:28" ht="34">
-      <c r="B70" s="186"/>
+      <c r="B70" s="195"/>
       <c r="C70" s="2" t="s">
         <v>18</v>
       </c>
@@ -8467,7 +8565,7 @@
       </c>
       <c r="K70" s="99"/>
       <c r="L70" s="25"/>
-      <c r="M70" s="186"/>
+      <c r="M70" s="195"/>
       <c r="N70" s="2" t="s">
         <v>18</v>
       </c>
@@ -8513,7 +8611,7 @@
       </c>
     </row>
     <row r="71" spans="2:28" ht="69" thickBot="1">
-      <c r="B71" s="186"/>
+      <c r="B71" s="195"/>
       <c r="C71" s="21" t="s">
         <v>19</v>
       </c>
@@ -8537,7 +8635,7 @@
         <v>3.0237792142338398</v>
       </c>
       <c r="K71" s="99"/>
-      <c r="M71" s="186"/>
+      <c r="M71" s="195"/>
       <c r="N71" s="21" t="s">
         <v>19</v>
       </c>
@@ -8626,7 +8724,7 @@
       </c>
     </row>
     <row r="73" spans="2:28">
-      <c r="B73" s="186" t="s">
+      <c r="B73" s="195" t="s">
         <v>39</v>
       </c>
       <c r="C73" s="20" t="s">
@@ -8652,7 +8750,7 @@
         <v>2.2233044052248219</v>
       </c>
       <c r="K73" s="99"/>
-      <c r="M73" s="186" t="s">
+      <c r="M73" s="195" t="s">
         <v>39</v>
       </c>
       <c r="N73" s="20" t="s">
@@ -8679,7 +8777,7 @@
       </c>
     </row>
     <row r="74" spans="2:28">
-      <c r="B74" s="186"/>
+      <c r="B74" s="195"/>
       <c r="C74" s="2" t="s">
         <v>17</v>
       </c>
@@ -8703,7 +8801,7 @@
         <v>2.0428535562277461</v>
       </c>
       <c r="K74" s="99"/>
-      <c r="M74" s="186"/>
+      <c r="M74" s="195"/>
       <c r="N74" s="2" t="s">
         <v>17</v>
       </c>
@@ -8728,7 +8826,7 @@
       </c>
     </row>
     <row r="75" spans="2:28">
-      <c r="B75" s="186"/>
+      <c r="B75" s="195"/>
       <c r="C75" s="2" t="s">
         <v>18</v>
       </c>
@@ -8753,7 +8851,7 @@
       </c>
       <c r="K75" s="99"/>
       <c r="L75" s="25"/>
-      <c r="M75" s="186"/>
+      <c r="M75" s="195"/>
       <c r="N75" s="2" t="s">
         <v>18</v>
       </c>
@@ -8778,7 +8876,7 @@
       </c>
     </row>
     <row r="76" spans="2:28" ht="17" thickBot="1">
-      <c r="B76" s="187"/>
+      <c r="B76" s="196"/>
       <c r="C76" s="18" t="s">
         <v>19</v>
       </c>
@@ -8802,7 +8900,7 @@
         <v>3.0193695028281384</v>
       </c>
       <c r="K76" s="99"/>
-      <c r="M76" s="187"/>
+      <c r="M76" s="196"/>
       <c r="N76" s="18" t="s">
         <v>19</v>
       </c>
@@ -8853,7 +8951,7 @@
     <row r="78" spans="2:28">
       <c r="D78" s="26"/>
       <c r="K78" s="99"/>
-      <c r="M78" s="171" t="s">
+      <c r="M78" s="213" t="s">
         <v>269</v>
       </c>
       <c r="N78" s="20" t="s">
@@ -8882,7 +8980,7 @@
     <row r="79" spans="2:28">
       <c r="D79" s="26"/>
       <c r="K79" s="99"/>
-      <c r="M79" s="172"/>
+      <c r="M79" s="214"/>
       <c r="N79" s="2" t="s">
         <v>17</v>
       </c>
@@ -8911,7 +9009,7 @@
         <v>47</v>
       </c>
       <c r="K80" s="99"/>
-      <c r="M80" s="172"/>
+      <c r="M80" s="214"/>
       <c r="N80" s="2" t="s">
         <v>18</v>
       </c>
@@ -8959,7 +9057,7 @@
         <v>25</v>
       </c>
       <c r="K81" s="99"/>
-      <c r="M81" s="173"/>
+      <c r="M81" s="215"/>
       <c r="N81" s="18" t="s">
         <v>19</v>
       </c>
@@ -8984,7 +9082,7 @@
       </c>
     </row>
     <row r="82" spans="2:20">
-      <c r="B82" s="183" t="s">
+      <c r="B82" s="191" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="20" t="s">
@@ -9012,7 +9110,7 @@
       <c r="K82" s="99"/>
     </row>
     <row r="83" spans="2:20">
-      <c r="B83" s="166"/>
+      <c r="B83" s="192"/>
       <c r="C83" s="2" t="s">
         <v>17</v>
       </c>
@@ -9038,7 +9136,7 @@
       <c r="K83" s="99"/>
     </row>
     <row r="84" spans="2:20">
-      <c r="B84" s="166"/>
+      <c r="B84" s="192"/>
       <c r="C84" s="2" t="s">
         <v>18</v>
       </c>
@@ -9064,7 +9162,7 @@
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="2:20" ht="17" thickBot="1">
-      <c r="B85" s="167"/>
+      <c r="B85" s="193"/>
       <c r="C85" s="18" t="s">
         <v>19</v>
       </c>
@@ -9113,7 +9211,7 @@
       <c r="K86" s="99"/>
     </row>
     <row r="87" spans="2:20" ht="17" thickBot="1">
-      <c r="B87" s="183" t="s">
+      <c r="B87" s="191" t="s">
         <v>36</v>
       </c>
       <c r="C87" s="20" t="s">
@@ -9144,7 +9242,7 @@
       </c>
     </row>
     <row r="88" spans="2:20" ht="17" thickBot="1">
-      <c r="B88" s="166"/>
+      <c r="B88" s="192"/>
       <c r="C88" s="2" t="s">
         <v>17</v>
       </c>
@@ -9192,7 +9290,7 @@
       </c>
     </row>
     <row r="89" spans="2:20" ht="17" thickBot="1">
-      <c r="B89" s="166"/>
+      <c r="B89" s="192"/>
       <c r="C89" s="2" t="s">
         <v>18</v>
       </c>
@@ -9216,7 +9314,7 @@
         <v>0.282491961308796</v>
       </c>
       <c r="K89" s="99"/>
-      <c r="M89" s="183" t="s">
+      <c r="M89" s="191" t="s">
         <v>15</v>
       </c>
       <c r="N89" s="20" t="s">
@@ -9243,7 +9341,7 @@
       </c>
     </row>
     <row r="90" spans="2:20" ht="17" thickBot="1">
-      <c r="B90" s="167"/>
+      <c r="B90" s="193"/>
       <c r="C90" s="18" t="s">
         <v>19</v>
       </c>
@@ -9268,7 +9366,7 @@
       </c>
       <c r="K90" s="99"/>
       <c r="L90" s="25"/>
-      <c r="M90" s="166"/>
+      <c r="M90" s="192"/>
       <c r="N90" s="2" t="s">
         <v>17</v>
       </c>
@@ -9314,7 +9412,7 @@
         <v>25</v>
       </c>
       <c r="K91" s="99"/>
-      <c r="M91" s="166"/>
+      <c r="M91" s="192"/>
       <c r="N91" s="2" t="s">
         <v>18</v>
       </c>
@@ -9339,7 +9437,7 @@
       </c>
     </row>
     <row r="92" spans="2:20" ht="17" thickBot="1">
-      <c r="B92" s="183" t="s">
+      <c r="B92" s="191" t="s">
         <v>38</v>
       </c>
       <c r="C92" s="20" t="s">
@@ -9366,7 +9464,7 @@
       </c>
       <c r="K92" s="99"/>
       <c r="L92" s="44"/>
-      <c r="M92" s="167"/>
+      <c r="M92" s="193"/>
       <c r="N92" s="18" t="s">
         <v>19</v>
       </c>
@@ -9391,7 +9489,7 @@
       </c>
     </row>
     <row r="93" spans="2:20" ht="17" thickBot="1">
-      <c r="B93" s="166"/>
+      <c r="B93" s="192"/>
       <c r="C93" s="2" t="s">
         <v>17</v>
       </c>
@@ -9438,7 +9536,7 @@
       </c>
     </row>
     <row r="94" spans="2:20" ht="17" thickBot="1">
-      <c r="B94" s="166"/>
+      <c r="B94" s="192"/>
       <c r="C94" s="2" t="s">
         <v>18</v>
       </c>
@@ -9463,7 +9561,7 @@
       </c>
       <c r="K94" s="99"/>
       <c r="L94" s="44"/>
-      <c r="M94" s="183" t="s">
+      <c r="M94" s="191" t="s">
         <v>36</v>
       </c>
       <c r="N94" s="20" t="s">
@@ -9490,7 +9588,7 @@
       </c>
     </row>
     <row r="95" spans="2:20" ht="17" thickBot="1">
-      <c r="B95" s="184"/>
+      <c r="B95" s="204"/>
       <c r="C95" s="21" t="s">
         <v>19</v>
       </c>
@@ -9515,7 +9613,7 @@
       </c>
       <c r="K95" s="99"/>
       <c r="L95" s="44"/>
-      <c r="M95" s="166"/>
+      <c r="M95" s="192"/>
       <c r="N95" s="2" t="s">
         <v>17</v>
       </c>
@@ -9562,7 +9660,7 @@
       </c>
       <c r="K96" s="99"/>
       <c r="L96" s="25"/>
-      <c r="M96" s="166"/>
+      <c r="M96" s="192"/>
       <c r="N96" s="2" t="s">
         <v>18</v>
       </c>
@@ -9587,7 +9685,7 @@
       </c>
     </row>
     <row r="97" spans="2:20" ht="17" thickBot="1">
-      <c r="B97" s="183" t="s">
+      <c r="B97" s="191" t="s">
         <v>39</v>
       </c>
       <c r="C97" s="20" t="s">
@@ -9614,7 +9712,7 @@
       </c>
       <c r="K97" s="99"/>
       <c r="L97" s="44"/>
-      <c r="M97" s="167"/>
+      <c r="M97" s="193"/>
       <c r="N97" s="18" t="s">
         <v>19</v>
       </c>
@@ -9639,7 +9737,7 @@
       </c>
     </row>
     <row r="98" spans="2:20" ht="17" thickBot="1">
-      <c r="B98" s="166"/>
+      <c r="B98" s="192"/>
       <c r="C98" s="2" t="s">
         <v>17</v>
       </c>
@@ -9686,7 +9784,7 @@
       </c>
     </row>
     <row r="99" spans="2:20" ht="17" thickBot="1">
-      <c r="B99" s="166"/>
+      <c r="B99" s="192"/>
       <c r="C99" s="2" t="s">
         <v>18</v>
       </c>
@@ -9711,7 +9809,7 @@
       </c>
       <c r="K99" s="99"/>
       <c r="L99" s="44"/>
-      <c r="M99" s="183" t="s">
+      <c r="M99" s="191" t="s">
         <v>38</v>
       </c>
       <c r="N99" s="20" t="s">
@@ -9738,7 +9836,7 @@
       </c>
     </row>
     <row r="100" spans="2:20" ht="17" thickBot="1">
-      <c r="B100" s="167"/>
+      <c r="B100" s="193"/>
       <c r="C100" s="18" t="s">
         <v>19</v>
       </c>
@@ -9763,7 +9861,7 @@
       </c>
       <c r="K100" s="99"/>
       <c r="L100" s="44"/>
-      <c r="M100" s="166"/>
+      <c r="M100" s="192"/>
       <c r="N100" s="2" t="s">
         <v>17</v>
       </c>
@@ -9810,7 +9908,7 @@
       </c>
       <c r="K101" s="99"/>
       <c r="L101" s="25"/>
-      <c r="M101" s="166"/>
+      <c r="M101" s="192"/>
       <c r="N101" s="2" t="s">
         <v>18</v>
       </c>
@@ -9835,7 +9933,7 @@
       </c>
     </row>
     <row r="102" spans="2:20" ht="17" thickBot="1">
-      <c r="B102" s="185" t="s">
+      <c r="B102" s="203" t="s">
         <v>57</v>
       </c>
       <c r="C102" s="48" t="s">
@@ -9862,7 +9960,7 @@
       </c>
       <c r="K102" s="99"/>
       <c r="L102" s="44"/>
-      <c r="M102" s="184"/>
+      <c r="M102" s="204"/>
       <c r="N102" s="21" t="s">
         <v>19</v>
       </c>
@@ -9887,7 +9985,7 @@
       </c>
     </row>
     <row r="103" spans="2:20" ht="17" thickBot="1">
-      <c r="B103" s="166"/>
+      <c r="B103" s="192"/>
       <c r="C103" s="2" t="s">
         <v>17</v>
       </c>
@@ -9934,7 +10032,7 @@
       </c>
     </row>
     <row r="104" spans="2:20" ht="17" thickBot="1">
-      <c r="B104" s="166"/>
+      <c r="B104" s="192"/>
       <c r="C104" s="2" t="s">
         <v>18</v>
       </c>
@@ -9959,7 +10057,7 @@
       </c>
       <c r="K104" s="99"/>
       <c r="L104" s="44"/>
-      <c r="M104" s="183" t="s">
+      <c r="M104" s="191" t="s">
         <v>39</v>
       </c>
       <c r="N104" s="20" t="s">
@@ -9986,7 +10084,7 @@
       </c>
     </row>
     <row r="105" spans="2:20" ht="17" thickBot="1">
-      <c r="B105" s="167"/>
+      <c r="B105" s="193"/>
       <c r="C105" s="18" t="s">
         <v>19</v>
       </c>
@@ -10011,7 +10109,7 @@
       </c>
       <c r="K105" s="99"/>
       <c r="L105" s="44"/>
-      <c r="M105" s="166"/>
+      <c r="M105" s="192"/>
       <c r="N105" s="2" t="s">
         <v>17</v>
       </c>
@@ -10038,7 +10136,7 @@
     <row r="106" spans="2:20" ht="17" thickBot="1">
       <c r="K106" s="99"/>
       <c r="L106" s="25"/>
-      <c r="M106" s="166"/>
+      <c r="M106" s="192"/>
       <c r="N106" s="2" t="s">
         <v>18</v>
       </c>
@@ -10066,7 +10164,7 @@
       <c r="D107" s="26"/>
       <c r="J107" s="60"/>
       <c r="K107" s="100"/>
-      <c r="M107" s="167"/>
+      <c r="M107" s="193"/>
       <c r="N107" s="18" t="s">
         <v>19</v>
       </c>
@@ -10117,7 +10215,7 @@
     <row r="109" spans="2:20" ht="17" thickBot="1">
       <c r="J109" s="57"/>
       <c r="K109" s="101"/>
-      <c r="M109" s="185" t="s">
+      <c r="M109" s="203" t="s">
         <v>57</v>
       </c>
       <c r="N109" s="48" t="s">
@@ -10146,7 +10244,7 @@
     <row r="110" spans="2:20" ht="17" thickBot="1">
       <c r="J110" s="57"/>
       <c r="K110" s="101"/>
-      <c r="M110" s="166"/>
+      <c r="M110" s="192"/>
       <c r="N110" s="2" t="s">
         <v>17</v>
       </c>
@@ -10173,7 +10271,7 @@
     <row r="111" spans="2:20" ht="17" thickBot="1">
       <c r="J111" s="60"/>
       <c r="K111" s="100"/>
-      <c r="M111" s="166"/>
+      <c r="M111" s="192"/>
       <c r="N111" s="2" t="s">
         <v>18</v>
       </c>
@@ -10201,7 +10299,7 @@
       <c r="D112" s="26"/>
       <c r="J112" s="57"/>
       <c r="K112" s="101"/>
-      <c r="M112" s="167"/>
+      <c r="M112" s="193"/>
       <c r="N112" s="18" t="s">
         <v>19</v>
       </c>
@@ -10252,7 +10350,7 @@
     <row r="114" spans="4:20" ht="17" thickBot="1">
       <c r="J114" s="57"/>
       <c r="K114" s="101"/>
-      <c r="M114" s="171" t="s">
+      <c r="M114" s="213" t="s">
         <v>214</v>
       </c>
       <c r="N114" s="20" t="s">
@@ -10281,7 +10379,7 @@
     <row r="115" spans="4:20" ht="17" thickBot="1">
       <c r="J115" s="60"/>
       <c r="K115" s="100"/>
-      <c r="M115" s="172"/>
+      <c r="M115" s="214"/>
       <c r="N115" s="2" t="s">
         <v>17</v>
       </c>
@@ -10308,7 +10406,7 @@
     <row r="116" spans="4:20" ht="17" thickBot="1">
       <c r="J116" s="57"/>
       <c r="K116" s="101"/>
-      <c r="M116" s="172"/>
+      <c r="M116" s="214"/>
       <c r="N116" s="2" t="s">
         <v>18</v>
       </c>
@@ -10336,7 +10434,7 @@
       <c r="D117" s="26"/>
       <c r="J117" s="57"/>
       <c r="K117" s="101"/>
-      <c r="M117" s="173"/>
+      <c r="M117" s="215"/>
       <c r="N117" s="18" t="s">
         <v>19</v>
       </c>
@@ -10387,7 +10485,7 @@
     <row r="119" spans="4:20" ht="17" thickBot="1">
       <c r="J119" s="60"/>
       <c r="K119" s="100"/>
-      <c r="M119" s="165" t="s">
+      <c r="M119" s="198" t="s">
         <v>216</v>
       </c>
       <c r="N119" s="48" t="s">
@@ -10416,7 +10514,7 @@
     <row r="120" spans="4:20" ht="17" thickBot="1">
       <c r="J120" s="57"/>
       <c r="K120" s="101"/>
-      <c r="M120" s="166"/>
+      <c r="M120" s="192"/>
       <c r="N120" s="2" t="s">
         <v>17</v>
       </c>
@@ -10443,7 +10541,7 @@
     <row r="121" spans="4:20" ht="17" thickBot="1">
       <c r="J121" s="57"/>
       <c r="K121" s="101"/>
-      <c r="M121" s="166"/>
+      <c r="M121" s="192"/>
       <c r="N121" s="2" t="s">
         <v>18</v>
       </c>
@@ -10471,7 +10569,7 @@
       <c r="D122" s="26"/>
       <c r="J122" s="57"/>
       <c r="K122" s="101"/>
-      <c r="M122" s="167"/>
+      <c r="M122" s="193"/>
       <c r="N122" s="18" t="s">
         <v>19</v>
       </c>
@@ -10522,7 +10620,7 @@
     <row r="124" spans="4:20" ht="17" thickBot="1">
       <c r="J124" s="57"/>
       <c r="K124" s="101"/>
-      <c r="M124" s="165" t="s">
+      <c r="M124" s="198" t="s">
         <v>227</v>
       </c>
       <c r="N124" s="48" t="s">
@@ -10547,7 +10645,7 @@
     <row r="125" spans="4:20" ht="17" thickBot="1">
       <c r="J125" s="57"/>
       <c r="K125" s="101"/>
-      <c r="M125" s="166"/>
+      <c r="M125" s="192"/>
       <c r="N125" s="2" t="s">
         <v>17</v>
       </c>
@@ -10570,7 +10668,7 @@
     <row r="126" spans="4:20" ht="17" thickBot="1">
       <c r="J126" s="57"/>
       <c r="K126" s="101"/>
-      <c r="M126" s="166"/>
+      <c r="M126" s="192"/>
       <c r="N126" s="2" t="s">
         <v>18</v>
       </c>
@@ -10594,7 +10692,7 @@
       <c r="J127" s="57"/>
       <c r="K127" s="101"/>
       <c r="L127" s="25"/>
-      <c r="M127" s="167"/>
+      <c r="M127" s="193"/>
       <c r="N127" s="18" t="s">
         <v>19</v>
       </c>
@@ -10643,7 +10741,7 @@
       <c r="J129" s="57"/>
       <c r="K129" s="101"/>
       <c r="L129" s="44"/>
-      <c r="M129" s="168" t="s">
+      <c r="M129" s="216" t="s">
         <v>258</v>
       </c>
       <c r="N129" s="48" t="s">
@@ -10673,7 +10771,7 @@
       <c r="J130" s="57"/>
       <c r="K130" s="101"/>
       <c r="L130" s="44"/>
-      <c r="M130" s="169"/>
+      <c r="M130" s="217"/>
       <c r="N130" s="2" t="s">
         <v>17</v>
       </c>
@@ -10701,7 +10799,7 @@
       <c r="J131" s="57"/>
       <c r="K131" s="101"/>
       <c r="L131" s="44"/>
-      <c r="M131" s="169"/>
+      <c r="M131" s="217"/>
       <c r="N131" s="2" t="s">
         <v>18</v>
       </c>
@@ -10729,7 +10827,7 @@
       <c r="J132" s="57"/>
       <c r="K132" s="101"/>
       <c r="L132" s="44"/>
-      <c r="M132" s="170"/>
+      <c r="M132" s="218"/>
       <c r="N132" s="18" t="s">
         <v>19</v>
       </c>
@@ -10782,7 +10880,7 @@
       <c r="J134" s="57"/>
       <c r="K134" s="101"/>
       <c r="L134" s="44"/>
-      <c r="M134" s="168" t="s">
+      <c r="M134" s="216" t="s">
         <v>259</v>
       </c>
       <c r="N134" s="48" t="s">
@@ -10812,7 +10910,7 @@
       <c r="J135" s="57"/>
       <c r="K135" s="101"/>
       <c r="L135" s="44"/>
-      <c r="M135" s="169"/>
+      <c r="M135" s="217"/>
       <c r="N135" s="2" t="s">
         <v>17</v>
       </c>
@@ -10840,7 +10938,7 @@
       <c r="J136" s="57"/>
       <c r="K136" s="101"/>
       <c r="L136" s="25"/>
-      <c r="M136" s="169"/>
+      <c r="M136" s="217"/>
       <c r="N136" s="2" t="s">
         <v>18</v>
       </c>
@@ -10868,7 +10966,7 @@
       <c r="J137" s="57"/>
       <c r="K137" s="101"/>
       <c r="L137" s="44"/>
-      <c r="M137" s="170"/>
+      <c r="M137" s="218"/>
       <c r="N137" s="18" t="s">
         <v>19</v>
       </c>
@@ -10921,7 +11019,7 @@
       <c r="J139" s="57"/>
       <c r="K139" s="101"/>
       <c r="L139" s="44"/>
-      <c r="M139" s="168" t="s">
+      <c r="M139" s="216" t="s">
         <v>260</v>
       </c>
       <c r="N139" s="48" t="s">
@@ -10951,7 +11049,7 @@
       <c r="J140" s="57"/>
       <c r="K140" s="101"/>
       <c r="L140" s="44"/>
-      <c r="M140" s="169"/>
+      <c r="M140" s="217"/>
       <c r="N140" s="2" t="s">
         <v>17</v>
       </c>
@@ -10977,7 +11075,7 @@
     </row>
     <row r="141" spans="10:20" ht="17" thickBot="1">
       <c r="K141" s="99"/>
-      <c r="M141" s="169"/>
+      <c r="M141" s="217"/>
       <c r="N141" s="2" t="s">
         <v>18</v>
       </c>
@@ -11003,7 +11101,7 @@
     </row>
     <row r="142" spans="10:20" ht="17" thickBot="1">
       <c r="K142" s="99"/>
-      <c r="M142" s="170"/>
+      <c r="M142" s="218"/>
       <c r="N142" s="18" t="s">
         <v>19</v>
       </c>
@@ -11086,16 +11184,16 @@
       <c r="K150" s="159"/>
     </row>
     <row r="151" spans="1:11" ht="20">
-      <c r="B151" s="247" t="s">
+      <c r="B151" s="166" t="s">
         <v>362</v>
       </c>
-      <c r="C151" s="247" t="s">
+      <c r="C151" s="166" t="s">
         <v>363</v>
       </c>
-      <c r="D151" s="247" t="s">
+      <c r="D151" s="166" t="s">
         <v>364</v>
       </c>
-      <c r="E151" s="247" t="s">
+      <c r="E151" s="166" t="s">
         <v>365</v>
       </c>
       <c r="K151" s="159"/>
@@ -11183,16 +11281,16 @@
       <c r="K157" s="159"/>
     </row>
     <row r="158" spans="1:11" ht="16" customHeight="1">
-      <c r="B158" s="247" t="s">
+      <c r="B158" s="166" t="s">
         <v>362</v>
       </c>
-      <c r="C158" s="247" t="s">
+      <c r="C158" s="166" t="s">
         <v>363</v>
       </c>
-      <c r="D158" s="247" t="s">
+      <c r="D158" s="166" t="s">
         <v>364</v>
       </c>
-      <c r="E158" s="247" t="s">
+      <c r="E158" s="166" t="s">
         <v>365</v>
       </c>
       <c r="K158" s="159"/>
@@ -11243,10 +11341,10 @@
       <c r="K161" s="159"/>
     </row>
     <row r="162" spans="2:11" ht="20">
-      <c r="B162" s="248"/>
-      <c r="C162" s="248"/>
-      <c r="D162" s="248"/>
-      <c r="E162" s="248"/>
+      <c r="B162" s="167"/>
+      <c r="C162" s="167"/>
+      <c r="D162" s="167"/>
+      <c r="E162" s="167"/>
       <c r="K162" s="159"/>
     </row>
     <row r="163" spans="2:11">
@@ -11518,25 +11616,55 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="T31:T33"/>
-    <mergeCell ref="AA23:AA26"/>
-    <mergeCell ref="V23:V26"/>
-    <mergeCell ref="Y23:Y25"/>
-    <mergeCell ref="V27:V30"/>
-    <mergeCell ref="Y27:Y29"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="T23:T25"/>
-    <mergeCell ref="T27:T29"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="M27:M30"/>
-    <mergeCell ref="Q27:Q29"/>
-    <mergeCell ref="M23:M26"/>
-    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="M124:M127"/>
+    <mergeCell ref="M129:M132"/>
+    <mergeCell ref="M134:M137"/>
+    <mergeCell ref="M139:M142"/>
+    <mergeCell ref="M114:M117"/>
+    <mergeCell ref="X49:AA49"/>
+    <mergeCell ref="V58:V61"/>
+    <mergeCell ref="V49:V50"/>
+    <mergeCell ref="W49:W50"/>
+    <mergeCell ref="M119:M122"/>
+    <mergeCell ref="M78:M81"/>
+    <mergeCell ref="M89:M92"/>
+    <mergeCell ref="M94:M97"/>
+    <mergeCell ref="M99:M102"/>
+    <mergeCell ref="M104:M107"/>
+    <mergeCell ref="M109:M112"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="M63:M66"/>
+    <mergeCell ref="M68:M71"/>
+    <mergeCell ref="M73:M76"/>
+    <mergeCell ref="V51:V54"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="G51:G54"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="M45:M48"/>
     <mergeCell ref="X39:Z39"/>
     <mergeCell ref="V41:V44"/>
@@ -11553,55 +11681,25 @@
     <mergeCell ref="V39:V40"/>
     <mergeCell ref="V31:V34"/>
     <mergeCell ref="M41:M44"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="G51:G54"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="X49:AA49"/>
-    <mergeCell ref="V58:V61"/>
-    <mergeCell ref="V49:V50"/>
-    <mergeCell ref="W49:W50"/>
-    <mergeCell ref="M119:M122"/>
-    <mergeCell ref="M78:M81"/>
-    <mergeCell ref="M89:M92"/>
-    <mergeCell ref="M94:M97"/>
-    <mergeCell ref="M99:M102"/>
-    <mergeCell ref="M104:M107"/>
-    <mergeCell ref="M109:M112"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="M63:M66"/>
-    <mergeCell ref="M68:M71"/>
-    <mergeCell ref="M73:M76"/>
-    <mergeCell ref="V51:V54"/>
-    <mergeCell ref="M124:M127"/>
-    <mergeCell ref="M129:M132"/>
-    <mergeCell ref="M134:M137"/>
-    <mergeCell ref="M139:M142"/>
-    <mergeCell ref="M114:M117"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="T23:T25"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="M27:M30"/>
+    <mergeCell ref="Q27:Q29"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="T31:T33"/>
+    <mergeCell ref="AA23:AA26"/>
+    <mergeCell ref="V23:V26"/>
+    <mergeCell ref="Y23:Y25"/>
+    <mergeCell ref="V27:V30"/>
+    <mergeCell ref="Y27:Y29"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
@@ -11618,8 +11716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0E8EF5-5245-C440-9E45-AB650B27E96E}">
   <dimension ref="B2:T84"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:G50"/>
+    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11655,17 +11753,17 @@
       <c r="T3" s="44"/>
     </row>
     <row r="4" spans="2:20" ht="17" customHeight="1" thickBot="1">
-      <c r="B4" s="228" t="s">
+      <c r="B4" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="230" t="s">
+      <c r="C4" s="224" t="s">
         <v>333</v>
       </c>
-      <c r="D4" s="222" t="s">
+      <c r="D4" s="236" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="223"/>
-      <c r="F4" s="224"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="237"/>
       <c r="K4" s="30" t="s">
         <v>13</v>
       </c>
@@ -11692,8 +11790,8 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="58" thickBot="1">
-      <c r="B5" s="229"/>
-      <c r="C5" s="231"/>
+      <c r="B5" s="223"/>
+      <c r="C5" s="225"/>
       <c r="D5" s="130" t="s">
         <v>252</v>
       </c>
@@ -11703,7 +11801,7 @@
       <c r="F5" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="K5" s="246" t="s">
+      <c r="K5" s="235" t="s">
         <v>304</v>
       </c>
       <c r="L5" s="119" t="s">
@@ -11730,7 +11828,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="18">
-      <c r="B6" s="232" t="s">
+      <c r="B6" s="226" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="133" t="s">
@@ -11745,7 +11843,7 @@
       <c r="F6" s="135">
         <v>0.10224074800000001</v>
       </c>
-      <c r="K6" s="166"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="117" t="s">
         <v>335</v>
       </c>
@@ -11770,7 +11868,7 @@
       </c>
     </row>
     <row r="7" spans="2:20" ht="18">
-      <c r="B7" s="232"/>
+      <c r="B7" s="226"/>
       <c r="C7" s="136" t="s">
         <v>335</v>
       </c>
@@ -11783,7 +11881,7 @@
       <c r="F7" s="138">
         <v>0.121107901</v>
       </c>
-      <c r="K7" s="166"/>
+      <c r="K7" s="192"/>
       <c r="L7" s="117" t="s">
         <v>336</v>
       </c>
@@ -11808,7 +11906,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" ht="19" thickBot="1">
-      <c r="B8" s="232"/>
+      <c r="B8" s="226"/>
       <c r="C8" s="136" t="s">
         <v>336</v>
       </c>
@@ -11821,7 +11919,7 @@
       <c r="F8" s="138">
         <v>3.8051438E-2</v>
       </c>
-      <c r="K8" s="184"/>
+      <c r="K8" s="204"/>
       <c r="L8" s="123" t="s">
         <v>337</v>
       </c>
@@ -11846,7 +11944,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" ht="19" thickBot="1">
-      <c r="B9" s="233"/>
+      <c r="B9" s="227"/>
       <c r="C9" s="139" t="s">
         <v>337</v>
       </c>
@@ -11859,7 +11957,7 @@
       <c r="F9" s="141">
         <v>0.16300196</v>
       </c>
-      <c r="K9" s="234" t="s">
+      <c r="K9" s="231" t="s">
         <v>332</v>
       </c>
       <c r="L9" s="124" t="s">
@@ -11886,7 +11984,7 @@
       </c>
     </row>
     <row r="10" spans="2:20" ht="19" thickBot="1">
-      <c r="B10" s="236" t="s">
+      <c r="B10" s="228" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="142" t="s">
@@ -11901,7 +11999,7 @@
       <c r="F10" s="144">
         <v>7.2184580999999998E-2</v>
       </c>
-      <c r="K10" s="186"/>
+      <c r="K10" s="195"/>
       <c r="L10" s="117" t="s">
         <v>335</v>
       </c>
@@ -11926,7 +12024,7 @@
       </c>
     </row>
     <row r="11" spans="2:20" ht="19" thickBot="1">
-      <c r="B11" s="237"/>
+      <c r="B11" s="229"/>
       <c r="C11" s="145" t="s">
         <v>335</v>
       </c>
@@ -11939,7 +12037,7 @@
       <c r="F11" s="147">
         <v>0.33822035900000003</v>
       </c>
-      <c r="K11" s="186"/>
+      <c r="K11" s="195"/>
       <c r="L11" s="117" t="s">
         <v>336</v>
       </c>
@@ -11964,7 +12062,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="19" thickBot="1">
-      <c r="B12" s="237"/>
+      <c r="B12" s="229"/>
       <c r="C12" s="145" t="s">
         <v>336</v>
       </c>
@@ -11977,7 +12075,7 @@
       <c r="F12" s="147">
         <v>0.12986613599999999</v>
       </c>
-      <c r="K12" s="187"/>
+      <c r="K12" s="196"/>
       <c r="L12" s="118" t="s">
         <v>337</v>
       </c>
@@ -12002,7 +12100,7 @@
       </c>
     </row>
     <row r="13" spans="2:20" ht="19" thickBot="1">
-      <c r="B13" s="245"/>
+      <c r="B13" s="230"/>
       <c r="C13" s="148" t="s">
         <v>337</v>
       </c>
@@ -12015,7 +12113,7 @@
       <c r="F13" s="150">
         <v>0.36942296299999999</v>
       </c>
-      <c r="K13" s="234" t="s">
+      <c r="K13" s="231" t="s">
         <v>344</v>
       </c>
       <c r="L13" s="124" t="s">
@@ -12042,7 +12140,7 @@
       </c>
     </row>
     <row r="14" spans="2:20" ht="19" thickBot="1">
-      <c r="B14" s="235" t="s">
+      <c r="B14" s="241" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="136" t="s">
@@ -12054,10 +12152,10 @@
       <c r="E14" s="134">
         <v>0.24519776400000001</v>
       </c>
-      <c r="F14" s="225" t="s">
+      <c r="F14" s="238" t="s">
         <v>354</v>
       </c>
-      <c r="K14" s="186"/>
+      <c r="K14" s="195"/>
       <c r="L14" s="117" t="s">
         <v>335</v>
       </c>
@@ -12082,7 +12180,7 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="19" thickBot="1">
-      <c r="B15" s="232"/>
+      <c r="B15" s="226"/>
       <c r="C15" s="136" t="s">
         <v>335</v>
       </c>
@@ -12092,8 +12190,8 @@
       <c r="E15" s="137">
         <v>0.17929769800000001</v>
       </c>
-      <c r="F15" s="226"/>
-      <c r="K15" s="186"/>
+      <c r="F15" s="239"/>
+      <c r="K15" s="195"/>
       <c r="L15" s="117" t="s">
         <v>336</v>
       </c>
@@ -12118,7 +12216,7 @@
       </c>
     </row>
     <row r="16" spans="2:20" ht="19" thickBot="1">
-      <c r="B16" s="232"/>
+      <c r="B16" s="226"/>
       <c r="C16" s="136" t="s">
         <v>336</v>
       </c>
@@ -12128,8 +12226,8 @@
       <c r="E16" s="137">
         <v>0.19465853299999999</v>
       </c>
-      <c r="F16" s="226"/>
-      <c r="K16" s="187"/>
+      <c r="F16" s="239"/>
+      <c r="K16" s="196"/>
       <c r="L16" s="118" t="s">
         <v>337</v>
       </c>
@@ -12154,7 +12252,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="19" thickBot="1">
-      <c r="B17" s="233"/>
+      <c r="B17" s="227"/>
       <c r="C17" s="139" t="s">
         <v>337</v>
       </c>
@@ -12164,8 +12262,8 @@
       <c r="E17" s="140">
         <v>0.37616676900000001</v>
       </c>
-      <c r="F17" s="227"/>
-      <c r="K17" s="216" t="s">
+      <c r="F17" s="240"/>
+      <c r="K17" s="232" t="s">
         <v>345</v>
       </c>
       <c r="L17" s="124" t="s">
@@ -12192,7 +12290,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="17" thickBot="1">
-      <c r="K18" s="217"/>
+      <c r="K18" s="233"/>
       <c r="L18" s="117" t="s">
         <v>335</v>
       </c>
@@ -12217,7 +12315,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="17" thickBot="1">
-      <c r="K19" s="217"/>
+      <c r="K19" s="233"/>
       <c r="L19" s="117" t="s">
         <v>336</v>
       </c>
@@ -12242,7 +12340,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="17" thickBot="1">
-      <c r="K20" s="218"/>
+      <c r="K20" s="234"/>
       <c r="L20" s="118" t="s">
         <v>337</v>
       </c>
@@ -12267,18 +12365,18 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="B21" s="228" t="s">
+      <c r="B21" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="230" t="s">
+      <c r="C21" s="224" t="s">
         <v>333</v>
       </c>
-      <c r="D21" s="222" t="s">
+      <c r="D21" s="236" t="s">
         <v>254</v>
       </c>
-      <c r="E21" s="224"/>
+      <c r="E21" s="237"/>
       <c r="F21" s="151"/>
-      <c r="K21" s="216" t="s">
+      <c r="K21" s="232" t="s">
         <v>350</v>
       </c>
       <c r="L21" s="119" t="s">
@@ -12305,8 +12403,8 @@
       </c>
     </row>
     <row r="22" spans="2:18" ht="58" thickBot="1">
-      <c r="B22" s="229"/>
-      <c r="C22" s="231"/>
+      <c r="B22" s="223"/>
+      <c r="C22" s="225"/>
       <c r="D22" s="130" t="s">
         <v>252</v>
       </c>
@@ -12314,7 +12412,7 @@
         <v>256</v>
       </c>
       <c r="F22" s="151"/>
-      <c r="K22" s="217"/>
+      <c r="K22" s="233"/>
       <c r="L22" s="117" t="s">
         <v>335</v>
       </c>
@@ -12339,7 +12437,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" ht="19" thickBot="1">
-      <c r="B23" s="232" t="s">
+      <c r="B23" s="226" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="133" t="s">
@@ -12352,7 +12450,7 @@
         <v>8.3276908999999996E-2</v>
       </c>
       <c r="F23" s="151"/>
-      <c r="K23" s="217"/>
+      <c r="K23" s="233"/>
       <c r="L23" s="117" t="s">
         <v>336</v>
       </c>
@@ -12377,7 +12475,7 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="19" thickBot="1">
-      <c r="B24" s="232"/>
+      <c r="B24" s="226"/>
       <c r="C24" s="136" t="s">
         <v>335</v>
       </c>
@@ -12388,7 +12486,7 @@
         <v>0.10163755100000001</v>
       </c>
       <c r="F24" s="151"/>
-      <c r="K24" s="218"/>
+      <c r="K24" s="234"/>
       <c r="L24" s="118" t="s">
         <v>337</v>
       </c>
@@ -12413,7 +12511,7 @@
       </c>
     </row>
     <row r="25" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="B25" s="232"/>
+      <c r="B25" s="226"/>
       <c r="C25" s="136" t="s">
         <v>336</v>
       </c>
@@ -12424,7 +12522,7 @@
         <v>2.9157569000000001E-2</v>
       </c>
       <c r="F25" s="151"/>
-      <c r="K25" s="216" t="s">
+      <c r="K25" s="232" t="s">
         <v>346</v>
       </c>
       <c r="L25" s="119" t="s">
@@ -12451,7 +12549,7 @@
       </c>
     </row>
     <row r="26" spans="2:18" ht="19" thickBot="1">
-      <c r="B26" s="233"/>
+      <c r="B26" s="227"/>
       <c r="C26" s="139" t="s">
         <v>337</v>
       </c>
@@ -12462,7 +12560,7 @@
         <v>0.13460002800000001</v>
       </c>
       <c r="F26" s="151"/>
-      <c r="K26" s="217"/>
+      <c r="K26" s="233"/>
       <c r="L26" s="117" t="s">
         <v>335</v>
       </c>
@@ -12487,7 +12585,7 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="19" thickBot="1">
-      <c r="B27" s="236" t="s">
+      <c r="B27" s="228" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="142" t="s">
@@ -12500,7 +12598,7 @@
         <v>7.9383789999999996E-2</v>
       </c>
       <c r="F27" s="151"/>
-      <c r="K27" s="217"/>
+      <c r="K27" s="233"/>
       <c r="L27" s="117" t="s">
         <v>336</v>
       </c>
@@ -12525,7 +12623,7 @@
       </c>
     </row>
     <row r="28" spans="2:18" ht="19" thickBot="1">
-      <c r="B28" s="237"/>
+      <c r="B28" s="229"/>
       <c r="C28" s="145" t="s">
         <v>335</v>
       </c>
@@ -12536,7 +12634,7 @@
         <v>0.118666853</v>
       </c>
       <c r="F28" s="151"/>
-      <c r="K28" s="218"/>
+      <c r="K28" s="234"/>
       <c r="L28" s="118" t="s">
         <v>337</v>
       </c>
@@ -12561,7 +12659,7 @@
       </c>
     </row>
     <row r="29" spans="2:18" ht="18">
-      <c r="B29" s="237"/>
+      <c r="B29" s="229"/>
       <c r="C29" s="145" t="s">
         <v>336</v>
       </c>
@@ -12582,7 +12680,7 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="2:18" ht="19" thickBot="1">
-      <c r="B30" s="245"/>
+      <c r="B30" s="230"/>
       <c r="C30" s="148" t="s">
         <v>337</v>
       </c>
@@ -12603,7 +12701,7 @@
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="2:18" ht="19" thickBot="1">
-      <c r="B31" s="235" t="s">
+      <c r="B31" s="241" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="136" t="s">
@@ -12612,7 +12710,7 @@
       <c r="D31" s="134">
         <v>0.190903462</v>
       </c>
-      <c r="E31" s="225" t="s">
+      <c r="E31" s="238" t="s">
         <v>354</v>
       </c>
       <c r="F31" s="151"/>
@@ -12628,14 +12726,14 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="2:18" ht="19" thickBot="1">
-      <c r="B32" s="232"/>
+      <c r="B32" s="226"/>
       <c r="C32" s="136" t="s">
         <v>335</v>
       </c>
       <c r="D32" s="137">
         <v>0.26741922000000001</v>
       </c>
-      <c r="E32" s="226"/>
+      <c r="E32" s="239"/>
       <c r="F32" s="151"/>
       <c r="K32" s="30" t="s">
         <v>13</v>
@@ -12661,16 +12759,16 @@
       </c>
     </row>
     <row r="33" spans="2:18" ht="19" thickBot="1">
-      <c r="B33" s="232"/>
+      <c r="B33" s="226"/>
       <c r="C33" s="136" t="s">
         <v>336</v>
       </c>
       <c r="D33" s="137">
         <v>0.17281497700000001</v>
       </c>
-      <c r="E33" s="226"/>
+      <c r="E33" s="239"/>
       <c r="F33" s="151"/>
-      <c r="K33" s="246" t="s">
+      <c r="K33" s="235" t="s">
         <v>304</v>
       </c>
       <c r="L33" s="119" t="s">
@@ -12697,16 +12795,16 @@
       </c>
     </row>
     <row r="34" spans="2:18" ht="19" thickBot="1">
-      <c r="B34" s="233"/>
+      <c r="B34" s="227"/>
       <c r="C34" s="139" t="s">
         <v>337</v>
       </c>
       <c r="D34" s="140">
         <v>0.39427188000000002</v>
       </c>
-      <c r="E34" s="227"/>
+      <c r="E34" s="240"/>
       <c r="F34" s="151"/>
-      <c r="K34" s="166"/>
+      <c r="K34" s="192"/>
       <c r="L34" s="117" t="s">
         <v>335</v>
       </c>
@@ -12736,7 +12834,7 @@
       <c r="D35" s="151"/>
       <c r="E35" s="151"/>
       <c r="F35" s="151"/>
-      <c r="K35" s="166"/>
+      <c r="K35" s="192"/>
       <c r="L35" s="117" t="s">
         <v>336</v>
       </c>
@@ -12766,7 +12864,7 @@
       <c r="D36" s="151"/>
       <c r="E36" s="151"/>
       <c r="F36" s="151"/>
-      <c r="K36" s="167"/>
+      <c r="K36" s="193"/>
       <c r="L36" s="118" t="s">
         <v>337</v>
       </c>
@@ -12791,19 +12889,19 @@
       </c>
     </row>
     <row r="37" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="B37" s="228" t="s">
+      <c r="B37" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="230" t="s">
+      <c r="C37" s="224" t="s">
         <v>333</v>
       </c>
-      <c r="D37" s="222" t="s">
+      <c r="D37" s="236" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="223"/>
-      <c r="F37" s="223"/>
-      <c r="G37" s="224"/>
-      <c r="K37" s="234" t="s">
+      <c r="E37" s="246"/>
+      <c r="F37" s="246"/>
+      <c r="G37" s="237"/>
+      <c r="K37" s="231" t="s">
         <v>332</v>
       </c>
       <c r="L37" s="119" t="s">
@@ -12830,8 +12928,8 @@
       </c>
     </row>
     <row r="38" spans="2:18" ht="41" thickBot="1">
-      <c r="B38" s="229"/>
-      <c r="C38" s="231"/>
+      <c r="B38" s="223"/>
+      <c r="C38" s="225"/>
       <c r="D38" s="130" t="s">
         <v>253</v>
       </c>
@@ -12844,7 +12942,7 @@
       <c r="G38" s="152" t="s">
         <v>355</v>
       </c>
-      <c r="K38" s="186"/>
+      <c r="K38" s="195"/>
       <c r="L38" s="117" t="s">
         <v>335</v>
       </c>
@@ -12869,7 +12967,7 @@
       </c>
     </row>
     <row r="39" spans="2:18" ht="19" thickBot="1">
-      <c r="B39" s="232" t="s">
+      <c r="B39" s="226" t="s">
         <v>10</v>
       </c>
       <c r="C39" s="133" t="s">
@@ -12884,10 +12982,10 @@
       <c r="F39" s="135">
         <v>0.73226722899999996</v>
       </c>
-      <c r="G39" s="242" t="s">
+      <c r="G39" s="247" t="s">
         <v>356</v>
       </c>
-      <c r="K39" s="186"/>
+      <c r="K39" s="195"/>
       <c r="L39" s="117" t="s">
         <v>336</v>
       </c>
@@ -12912,7 +13010,7 @@
       </c>
     </row>
     <row r="40" spans="2:18" ht="19" thickBot="1">
-      <c r="B40" s="232"/>
+      <c r="B40" s="226"/>
       <c r="C40" s="136" t="s">
         <v>335</v>
       </c>
@@ -12925,8 +13023,8 @@
       <c r="F40" s="138">
         <v>0.49588315500000002</v>
       </c>
-      <c r="G40" s="243"/>
-      <c r="K40" s="187"/>
+      <c r="G40" s="248"/>
+      <c r="K40" s="196"/>
       <c r="L40" s="118" t="s">
         <v>337</v>
       </c>
@@ -12951,7 +13049,7 @@
       </c>
     </row>
     <row r="41" spans="2:18" ht="19" thickBot="1">
-      <c r="B41" s="232"/>
+      <c r="B41" s="226"/>
       <c r="C41" s="136" t="s">
         <v>336</v>
       </c>
@@ -12964,8 +13062,8 @@
       <c r="F41" s="138">
         <v>0.28808858799999998</v>
       </c>
-      <c r="G41" s="243"/>
-      <c r="K41" s="234" t="s">
+      <c r="G41" s="248"/>
+      <c r="K41" s="231" t="s">
         <v>344</v>
       </c>
       <c r="L41" s="119" t="s">
@@ -12992,7 +13090,7 @@
       </c>
     </row>
     <row r="42" spans="2:18" ht="19" thickBot="1">
-      <c r="B42" s="233"/>
+      <c r="B42" s="227"/>
       <c r="C42" s="139" t="s">
         <v>337</v>
       </c>
@@ -13005,8 +13103,8 @@
       <c r="F42" s="141">
         <v>0.93048497100000005</v>
       </c>
-      <c r="G42" s="243"/>
-      <c r="K42" s="186"/>
+      <c r="G42" s="248"/>
+      <c r="K42" s="195"/>
       <c r="L42" s="117" t="s">
         <v>335</v>
       </c>
@@ -13031,7 +13129,7 @@
       </c>
     </row>
     <row r="43" spans="2:18" ht="19" thickBot="1">
-      <c r="B43" s="236" t="s">
+      <c r="B43" s="228" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="142" t="s">
@@ -13046,8 +13144,8 @@
       <c r="F43" s="144">
         <v>0.73510694799999998</v>
       </c>
-      <c r="G43" s="243"/>
-      <c r="K43" s="186"/>
+      <c r="G43" s="248"/>
+      <c r="K43" s="195"/>
       <c r="L43" s="117" t="s">
         <v>336</v>
       </c>
@@ -13072,7 +13170,7 @@
       </c>
     </row>
     <row r="44" spans="2:18" ht="19" thickBot="1">
-      <c r="B44" s="237"/>
+      <c r="B44" s="229"/>
       <c r="C44" s="145" t="s">
         <v>335</v>
       </c>
@@ -13085,8 +13183,8 @@
       <c r="F44" s="147">
         <v>0.375448901</v>
       </c>
-      <c r="G44" s="243"/>
-      <c r="K44" s="187"/>
+      <c r="G44" s="248"/>
+      <c r="K44" s="196"/>
       <c r="L44" s="118" t="s">
         <v>337</v>
       </c>
@@ -13111,7 +13209,7 @@
       </c>
     </row>
     <row r="45" spans="2:18" ht="19" thickBot="1">
-      <c r="B45" s="237"/>
+      <c r="B45" s="229"/>
       <c r="C45" s="145" t="s">
         <v>336</v>
       </c>
@@ -13124,8 +13222,8 @@
       <c r="F45" s="147">
         <v>0.511421024</v>
       </c>
-      <c r="G45" s="243"/>
-      <c r="K45" s="216" t="s">
+      <c r="G45" s="248"/>
+      <c r="K45" s="232" t="s">
         <v>345</v>
       </c>
       <c r="L45" s="119" t="s">
@@ -13152,7 +13250,7 @@
       </c>
     </row>
     <row r="46" spans="2:18" ht="19" thickBot="1">
-      <c r="B46" s="238"/>
+      <c r="B46" s="242"/>
       <c r="C46" s="153" t="s">
         <v>337</v>
       </c>
@@ -13165,8 +13263,8 @@
       <c r="F46" s="155">
         <v>0.97103789200000001</v>
       </c>
-      <c r="G46" s="243"/>
-      <c r="K46" s="217"/>
+      <c r="G46" s="248"/>
+      <c r="K46" s="233"/>
       <c r="L46" s="117" t="s">
         <v>335</v>
       </c>
@@ -13191,7 +13289,7 @@
       </c>
     </row>
     <row r="47" spans="2:18" ht="19" thickBot="1">
-      <c r="B47" s="235" t="s">
+      <c r="B47" s="241" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="156" t="s">
@@ -13203,11 +13301,11 @@
       <c r="E47" s="157">
         <v>0.181299869</v>
       </c>
-      <c r="F47" s="239" t="s">
+      <c r="F47" s="243" t="s">
         <v>354</v>
       </c>
-      <c r="G47" s="243"/>
-      <c r="K47" s="217"/>
+      <c r="G47" s="248"/>
+      <c r="K47" s="233"/>
       <c r="L47" s="117" t="s">
         <v>336</v>
       </c>
@@ -13232,7 +13330,7 @@
       </c>
     </row>
     <row r="48" spans="2:18" ht="19" thickBot="1">
-      <c r="B48" s="232"/>
+      <c r="B48" s="226"/>
       <c r="C48" s="136" t="s">
         <v>335</v>
       </c>
@@ -13242,9 +13340,9 @@
       <c r="E48" s="137">
         <v>0.208914723</v>
       </c>
-      <c r="F48" s="240"/>
-      <c r="G48" s="243"/>
-      <c r="K48" s="218"/>
+      <c r="F48" s="244"/>
+      <c r="G48" s="248"/>
+      <c r="K48" s="234"/>
       <c r="L48" s="118" t="s">
         <v>337</v>
       </c>
@@ -13269,7 +13367,7 @@
       </c>
     </row>
     <row r="49" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="B49" s="232"/>
+      <c r="B49" s="226"/>
       <c r="C49" s="136" t="s">
         <v>336</v>
       </c>
@@ -13279,9 +13377,9 @@
       <c r="E49" s="137">
         <v>0.14118196899999999</v>
       </c>
-      <c r="F49" s="240"/>
-      <c r="G49" s="243"/>
-      <c r="K49" s="216" t="s">
+      <c r="F49" s="244"/>
+      <c r="G49" s="248"/>
+      <c r="K49" s="232" t="s">
         <v>350</v>
       </c>
       <c r="L49" s="119" t="s">
@@ -13308,7 +13406,7 @@
       </c>
     </row>
     <row r="50" spans="2:18" ht="19" thickBot="1">
-      <c r="B50" s="233"/>
+      <c r="B50" s="227"/>
       <c r="C50" s="139" t="s">
         <v>337</v>
       </c>
@@ -13318,9 +13416,9 @@
       <c r="E50" s="158">
         <v>0.310617427</v>
       </c>
-      <c r="F50" s="241"/>
-      <c r="G50" s="244"/>
-      <c r="K50" s="217"/>
+      <c r="F50" s="245"/>
+      <c r="G50" s="249"/>
+      <c r="K50" s="233"/>
       <c r="L50" s="117" t="s">
         <v>335</v>
       </c>
@@ -13345,7 +13443,7 @@
       </c>
     </row>
     <row r="51" spans="2:18" ht="17" thickBot="1">
-      <c r="K51" s="217"/>
+      <c r="K51" s="233"/>
       <c r="L51" s="117" t="s">
         <v>336</v>
       </c>
@@ -13370,7 +13468,7 @@
       </c>
     </row>
     <row r="52" spans="2:18" ht="17" thickBot="1">
-      <c r="K52" s="218"/>
+      <c r="K52" s="234"/>
       <c r="L52" s="118" t="s">
         <v>337</v>
       </c>
@@ -13395,7 +13493,7 @@
       </c>
     </row>
     <row r="53" spans="2:18" ht="17" customHeight="1" thickBot="1">
-      <c r="K53" s="216" t="s">
+      <c r="K53" s="232" t="s">
         <v>346</v>
       </c>
       <c r="L53" s="119" t="s">
@@ -13422,7 +13520,7 @@
       </c>
     </row>
     <row r="54" spans="2:18" ht="17" thickBot="1">
-      <c r="K54" s="217"/>
+      <c r="K54" s="233"/>
       <c r="L54" s="117" t="s">
         <v>335</v>
       </c>
@@ -13447,7 +13545,7 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="17" thickBot="1">
-      <c r="K55" s="217"/>
+      <c r="K55" s="233"/>
       <c r="L55" s="117" t="s">
         <v>336</v>
       </c>
@@ -13472,7 +13570,7 @@
       </c>
     </row>
     <row r="56" spans="2:18" ht="17" thickBot="1">
-      <c r="K56" s="218"/>
+      <c r="K56" s="234"/>
       <c r="L56" s="118" t="s">
         <v>337</v>
       </c>
@@ -13553,7 +13651,7 @@
       </c>
     </row>
     <row r="61" spans="2:18" ht="17" thickBot="1">
-      <c r="K61" s="246" t="s">
+      <c r="K61" s="235" t="s">
         <v>304</v>
       </c>
       <c r="L61" s="119" t="s">
@@ -13580,7 +13678,7 @@
       </c>
     </row>
     <row r="62" spans="2:18" ht="17" thickBot="1">
-      <c r="K62" s="166"/>
+      <c r="K62" s="192"/>
       <c r="L62" s="117" t="s">
         <v>335</v>
       </c>
@@ -13605,7 +13703,7 @@
       </c>
     </row>
     <row r="63" spans="2:18" ht="17" thickBot="1">
-      <c r="K63" s="166"/>
+      <c r="K63" s="192"/>
       <c r="L63" s="117" t="s">
         <v>336</v>
       </c>
@@ -13630,7 +13728,7 @@
       </c>
     </row>
     <row r="64" spans="2:18" ht="17" thickBot="1">
-      <c r="K64" s="167"/>
+      <c r="K64" s="193"/>
       <c r="L64" s="118" t="s">
         <v>337</v>
       </c>
@@ -13655,7 +13753,7 @@
       </c>
     </row>
     <row r="65" spans="11:18" ht="17" thickBot="1">
-      <c r="K65" s="234" t="s">
+      <c r="K65" s="231" t="s">
         <v>332</v>
       </c>
       <c r="L65" s="119" t="s">
@@ -13682,7 +13780,7 @@
       </c>
     </row>
     <row r="66" spans="11:18" ht="17" thickBot="1">
-      <c r="K66" s="186"/>
+      <c r="K66" s="195"/>
       <c r="L66" s="117" t="s">
         <v>335</v>
       </c>
@@ -13703,7 +13801,7 @@
       </c>
     </row>
     <row r="67" spans="11:18" ht="17" thickBot="1">
-      <c r="K67" s="186"/>
+      <c r="K67" s="195"/>
       <c r="L67" s="117" t="s">
         <v>336</v>
       </c>
@@ -13724,7 +13822,7 @@
       </c>
     </row>
     <row r="68" spans="11:18" ht="17" thickBot="1">
-      <c r="K68" s="187"/>
+      <c r="K68" s="196"/>
       <c r="L68" s="118" t="s">
         <v>337</v>
       </c>
@@ -13745,7 +13843,7 @@
       </c>
     </row>
     <row r="69" spans="11:18">
-      <c r="K69" s="234" t="s">
+      <c r="K69" s="231" t="s">
         <v>344</v>
       </c>
       <c r="L69" s="119" t="s">
@@ -13769,7 +13867,7 @@
       <c r="R69" s="120"/>
     </row>
     <row r="70" spans="11:18">
-      <c r="K70" s="186"/>
+      <c r="K70" s="195"/>
       <c r="L70" s="117" t="s">
         <v>335</v>
       </c>
@@ -13781,7 +13879,7 @@
       <c r="R70" s="121"/>
     </row>
     <row r="71" spans="11:18">
-      <c r="K71" s="186"/>
+      <c r="K71" s="195"/>
       <c r="L71" s="117" t="s">
         <v>336</v>
       </c>
@@ -13793,7 +13891,7 @@
       <c r="R71" s="121"/>
     </row>
     <row r="72" spans="11:18" ht="17" thickBot="1">
-      <c r="K72" s="187"/>
+      <c r="K72" s="196"/>
       <c r="L72" s="118" t="s">
         <v>337</v>
       </c>
@@ -13805,7 +13903,7 @@
       <c r="R72" s="122"/>
     </row>
     <row r="73" spans="11:18" ht="17" thickBot="1">
-      <c r="K73" s="216" t="s">
+      <c r="K73" s="232" t="s">
         <v>345</v>
       </c>
       <c r="L73" s="124" t="s">
@@ -13832,7 +13930,7 @@
       </c>
     </row>
     <row r="74" spans="11:18" ht="17" thickBot="1">
-      <c r="K74" s="217"/>
+      <c r="K74" s="233"/>
       <c r="L74" s="117" t="s">
         <v>335</v>
       </c>
@@ -13857,7 +13955,7 @@
       </c>
     </row>
     <row r="75" spans="11:18" ht="17" thickBot="1">
-      <c r="K75" s="217"/>
+      <c r="K75" s="233"/>
       <c r="L75" s="117" t="s">
         <v>336</v>
       </c>
@@ -13882,7 +13980,7 @@
       </c>
     </row>
     <row r="76" spans="11:18" ht="17" thickBot="1">
-      <c r="K76" s="218"/>
+      <c r="K76" s="234"/>
       <c r="L76" s="118" t="s">
         <v>337</v>
       </c>
@@ -13907,7 +14005,7 @@
       </c>
     </row>
     <row r="77" spans="11:18" ht="17" customHeight="1" thickBot="1">
-      <c r="K77" s="216" t="s">
+      <c r="K77" s="232" t="s">
         <v>350</v>
       </c>
       <c r="L77" s="119" t="s">
@@ -13934,7 +14032,7 @@
       </c>
     </row>
     <row r="78" spans="11:18" ht="17" thickBot="1">
-      <c r="K78" s="217"/>
+      <c r="K78" s="233"/>
       <c r="L78" s="117" t="s">
         <v>335</v>
       </c>
@@ -13959,7 +14057,7 @@
       </c>
     </row>
     <row r="79" spans="11:18" ht="17" thickBot="1">
-      <c r="K79" s="217"/>
+      <c r="K79" s="233"/>
       <c r="L79" s="117" t="s">
         <v>336</v>
       </c>
@@ -13984,7 +14082,7 @@
       </c>
     </row>
     <row r="80" spans="11:18" ht="17" thickBot="1">
-      <c r="K80" s="218"/>
+      <c r="K80" s="234"/>
       <c r="L80" s="118" t="s">
         <v>337</v>
       </c>
@@ -14009,7 +14107,7 @@
       </c>
     </row>
     <row r="81" spans="11:18" ht="17" thickBot="1">
-      <c r="K81" s="216" t="s">
+      <c r="K81" s="232" t="s">
         <v>346</v>
       </c>
       <c r="L81" s="119" t="s">
@@ -14036,7 +14134,7 @@
       </c>
     </row>
     <row r="82" spans="11:18" ht="17" thickBot="1">
-      <c r="K82" s="217"/>
+      <c r="K82" s="233"/>
       <c r="L82" s="117" t="s">
         <v>335</v>
       </c>
@@ -14053,7 +14151,7 @@
       </c>
     </row>
     <row r="83" spans="11:18" ht="17" thickBot="1">
-      <c r="K83" s="217"/>
+      <c r="K83" s="233"/>
       <c r="L83" s="117" t="s">
         <v>336</v>
       </c>
@@ -14070,7 +14168,7 @@
       </c>
     </row>
     <row r="84" spans="11:18" ht="17" thickBot="1">
-      <c r="K84" s="218"/>
+      <c r="K84" s="234"/>
       <c r="L84" s="118" t="s">
         <v>337</v>
       </c>
@@ -14088,6 +14186,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="K81:K84"/>
+    <mergeCell ref="M81:M84"/>
+    <mergeCell ref="N81:N84"/>
+    <mergeCell ref="O81:O84"/>
+    <mergeCell ref="Q81:Q84"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="K73:K76"/>
+    <mergeCell ref="K77:K80"/>
+    <mergeCell ref="M69:M72"/>
+    <mergeCell ref="K13:K16"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="F47:F50"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="K53:K56"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="G39:G50"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="K37:K40"/>
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="O69:O72"/>
     <mergeCell ref="P69:P72"/>
     <mergeCell ref="Q69:Q72"/>
@@ -14104,41 +14237,6 @@
     <mergeCell ref="K65:K68"/>
     <mergeCell ref="M65:M68"/>
     <mergeCell ref="N65:N68"/>
-    <mergeCell ref="K37:K40"/>
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="K73:K76"/>
-    <mergeCell ref="K77:K80"/>
-    <mergeCell ref="M69:M72"/>
-    <mergeCell ref="K13:K16"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="K17:K20"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="F47:F50"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="K53:K56"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="G39:G50"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="K81:K84"/>
-    <mergeCell ref="M81:M84"/>
-    <mergeCell ref="N81:N84"/>
-    <mergeCell ref="O81:O84"/>
-    <mergeCell ref="Q81:Q84"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14149,8 +14247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B492611-C3D3-2F4E-BA77-111D2947681F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:H18"/>
+    <sheetView topLeftCell="S1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="AT104" sqref="AT104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14158,4 +14256,958 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC15348-14AB-3446-BEEE-2416A3592279}">
+  <dimension ref="B1:U49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.83203125" customWidth="1"/>
+    <col min="19" max="19" width="16.83203125" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21">
+      <c r="H1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" ht="17" thickBot="1"/>
+    <row r="3" spans="2:21" ht="18" customHeight="1">
+      <c r="B3" s="222" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="224" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" s="250"/>
+      <c r="E3" s="250" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="251"/>
+      <c r="H3" s="257" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="258" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="259"/>
+      <c r="K3" s="260"/>
+      <c r="O3" s="265" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="267" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q3" s="236" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="237"/>
+      <c r="S3" s="269" t="s">
+        <v>351</v>
+      </c>
+      <c r="T3" s="270"/>
+      <c r="U3" s="250" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="40" customHeight="1" thickBot="1">
+      <c r="B4" s="223"/>
+      <c r="C4" s="225"/>
+      <c r="D4" s="130" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="165" t="s">
+        <v>347</v>
+      </c>
+      <c r="F4" s="132" t="s">
+        <v>348</v>
+      </c>
+      <c r="H4" s="261"/>
+      <c r="I4" s="262" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="263" t="s">
+        <v>347</v>
+      </c>
+      <c r="K4" s="264" t="s">
+        <v>348</v>
+      </c>
+      <c r="O4" s="266"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="165" t="s">
+        <v>347</v>
+      </c>
+      <c r="R4" s="132" t="s">
+        <v>348</v>
+      </c>
+      <c r="S4" s="130" t="s">
+        <v>352</v>
+      </c>
+      <c r="T4" s="152" t="s">
+        <v>353</v>
+      </c>
+      <c r="U4" s="152" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="19" thickBot="1">
+      <c r="B5" s="226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="133" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="134">
+        <v>8.2978075999999998E-2</v>
+      </c>
+      <c r="E5" s="134">
+        <v>8.8694037000000003E-2</v>
+      </c>
+      <c r="F5" s="135">
+        <v>0.10224074800000001</v>
+      </c>
+      <c r="H5" s="252" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="J5" s="140">
+        <v>0.132523745</v>
+      </c>
+      <c r="K5" s="141">
+        <v>0.16300196</v>
+      </c>
+      <c r="O5" s="252" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="Q5" s="140">
+        <v>0.132523745</v>
+      </c>
+      <c r="R5" s="141">
+        <v>0.16300196</v>
+      </c>
+      <c r="S5" s="141">
+        <v>0.13796243799999999</v>
+      </c>
+      <c r="T5" s="141">
+        <v>0.93048497100000005</v>
+      </c>
+      <c r="U5" s="141">
+        <v>0.13460002800000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="19" thickBot="1">
+      <c r="B6" s="226"/>
+      <c r="C6" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6" s="137">
+        <v>9.9679073000000007E-2</v>
+      </c>
+      <c r="E6" s="137">
+        <v>9.3619396999999993E-2</v>
+      </c>
+      <c r="F6" s="138">
+        <v>0.121107901</v>
+      </c>
+      <c r="H6" s="253" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="149">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="J6" s="149">
+        <v>0.24602358899999999</v>
+      </c>
+      <c r="K6" s="150">
+        <v>0.36942296299999999</v>
+      </c>
+      <c r="O6" s="253" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="149">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="Q6" s="149">
+        <v>0.24602358899999999</v>
+      </c>
+      <c r="R6" s="150">
+        <v>0.36942296299999999</v>
+      </c>
+      <c r="S6" s="155">
+        <v>0.25645743100000001</v>
+      </c>
+      <c r="T6" s="155">
+        <v>0.97103789200000001</v>
+      </c>
+      <c r="U6" s="150">
+        <v>0.211236021</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="19" thickBot="1">
+      <c r="B7" s="226"/>
+      <c r="C7" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D7" s="137">
+        <v>2.9346153E-2</v>
+      </c>
+      <c r="E7" s="137">
+        <v>3.0510583000000001E-2</v>
+      </c>
+      <c r="F7" s="138">
+        <v>3.8051438E-2</v>
+      </c>
+      <c r="H7" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="J7" s="140">
+        <v>0.37616676900000001</v>
+      </c>
+      <c r="K7" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="O7" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="Q7" s="140">
+        <v>0.37616676900000001</v>
+      </c>
+      <c r="R7" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="S7" s="158">
+        <v>0.310617427</v>
+      </c>
+      <c r="T7" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="U7" s="140" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="19" thickBot="1">
+      <c r="B8" s="227"/>
+      <c r="C8" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="E8" s="140">
+        <v>0.132523745</v>
+      </c>
+      <c r="F8" s="141">
+        <v>0.16300196</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" ht="19" thickBot="1">
+      <c r="B9" s="228" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="142" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" s="143">
+        <v>8.6425494000000005E-2</v>
+      </c>
+      <c r="E9" s="143">
+        <v>9.0765129E-2</v>
+      </c>
+      <c r="F9" s="144">
+        <v>7.2184580999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" ht="18">
+      <c r="B10" s="229"/>
+      <c r="C10" s="145" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="146">
+        <v>0.109670028</v>
+      </c>
+      <c r="E10" s="146">
+        <v>0.19792855300000001</v>
+      </c>
+      <c r="F10" s="147">
+        <v>0.33822035900000003</v>
+      </c>
+      <c r="H10" s="222" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="236" t="s">
+        <v>254</v>
+      </c>
+      <c r="J10" s="237"/>
+    </row>
+    <row r="11" spans="2:21" ht="39" thickBot="1">
+      <c r="B11" s="229"/>
+      <c r="C11" s="145" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="146">
+        <v>0.16404260400000001</v>
+      </c>
+      <c r="E11" s="146">
+        <v>0.111279383</v>
+      </c>
+      <c r="F11" s="147">
+        <v>0.12986613599999999</v>
+      </c>
+      <c r="H11" s="223"/>
+      <c r="I11" s="130" t="s">
+        <v>252</v>
+      </c>
+      <c r="J11" s="152" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="19" thickBot="1">
+      <c r="B12" s="230"/>
+      <c r="C12" s="148" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="149">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="E12" s="149">
+        <v>0.24602358899999999</v>
+      </c>
+      <c r="F12" s="150">
+        <v>0.36942296299999999</v>
+      </c>
+      <c r="H12" s="252" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="J12" s="141">
+        <v>0.13460002800000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" ht="19" thickBot="1">
+      <c r="B13" s="241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="D13" s="134">
+        <v>0.190903462</v>
+      </c>
+      <c r="E13" s="134">
+        <v>0.24519776400000001</v>
+      </c>
+      <c r="F13" s="238" t="s">
+        <v>354</v>
+      </c>
+      <c r="H13" s="253" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="149">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="J13" s="150">
+        <v>0.211236021</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" ht="19" thickBot="1">
+      <c r="B14" s="226"/>
+      <c r="C14" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" s="137">
+        <v>0.26741922000000001</v>
+      </c>
+      <c r="E14" s="137">
+        <v>0.17929769800000001</v>
+      </c>
+      <c r="F14" s="239"/>
+      <c r="H14" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="J14" s="140" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="18">
+      <c r="B15" s="226"/>
+      <c r="C15" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D15" s="137">
+        <v>0.17281497700000001</v>
+      </c>
+      <c r="E15" s="137">
+        <v>0.19465853299999999</v>
+      </c>
+      <c r="F15" s="239"/>
+    </row>
+    <row r="16" spans="2:21" ht="19" thickBot="1">
+      <c r="B16" s="227"/>
+      <c r="C16" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="E16" s="140">
+        <v>0.37616676900000001</v>
+      </c>
+      <c r="F16" s="240"/>
+    </row>
+    <row r="17" spans="2:12" ht="17" thickBot="1"/>
+    <row r="18" spans="2:12" ht="18">
+      <c r="H18" s="222" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="236" t="s">
+        <v>351</v>
+      </c>
+      <c r="J18" s="246"/>
+      <c r="K18" s="246"/>
+      <c r="L18" s="237"/>
+    </row>
+    <row r="19" spans="2:12" ht="60" thickBot="1">
+      <c r="H19" s="223"/>
+      <c r="I19" s="130" t="s">
+        <v>252</v>
+      </c>
+      <c r="J19" s="130" t="s">
+        <v>352</v>
+      </c>
+      <c r="K19" s="152" t="s">
+        <v>353</v>
+      </c>
+      <c r="L19" s="152" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="19" customHeight="1" thickBot="1">
+      <c r="B20" s="222" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="224" t="s">
+        <v>333</v>
+      </c>
+      <c r="D20" s="236" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="237"/>
+      <c r="F20" s="151"/>
+      <c r="H20" s="252" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="J20" s="141">
+        <v>0.13796243799999999</v>
+      </c>
+      <c r="K20" s="141">
+        <v>0.93048497100000005</v>
+      </c>
+      <c r="L20" s="247" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="77" thickBot="1">
+      <c r="B21" s="223"/>
+      <c r="C21" s="225"/>
+      <c r="D21" s="130" t="s">
+        <v>252</v>
+      </c>
+      <c r="E21" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="F21" s="151"/>
+      <c r="H21" s="253" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="154">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="J21" s="155">
+        <v>0.25645743100000001</v>
+      </c>
+      <c r="K21" s="155">
+        <v>0.97103789200000001</v>
+      </c>
+      <c r="L21" s="255"/>
+    </row>
+    <row r="22" spans="2:12" ht="19" thickBot="1">
+      <c r="B22" s="226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="133" t="s">
+        <v>334</v>
+      </c>
+      <c r="D22" s="134">
+        <v>8.2978075999999998E-2</v>
+      </c>
+      <c r="E22" s="135">
+        <v>8.3276908999999996E-2</v>
+      </c>
+      <c r="F22" s="151"/>
+      <c r="H22" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="J22" s="158">
+        <v>0.310617427</v>
+      </c>
+      <c r="K22" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="L22" s="256"/>
+    </row>
+    <row r="23" spans="2:12" ht="18">
+      <c r="B23" s="226"/>
+      <c r="C23" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D23" s="137">
+        <v>9.9679073000000007E-2</v>
+      </c>
+      <c r="E23" s="138">
+        <v>0.10163755100000001</v>
+      </c>
+      <c r="F23" s="151"/>
+    </row>
+    <row r="24" spans="2:12" ht="18">
+      <c r="B24" s="226"/>
+      <c r="C24" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" s="137">
+        <v>2.9346153E-2</v>
+      </c>
+      <c r="E24" s="138">
+        <v>2.9157569000000001E-2</v>
+      </c>
+      <c r="F24" s="151"/>
+    </row>
+    <row r="25" spans="2:12" ht="19" thickBot="1">
+      <c r="B25" s="227"/>
+      <c r="C25" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="E25" s="141">
+        <v>0.13460002800000001</v>
+      </c>
+      <c r="F25" s="151"/>
+    </row>
+    <row r="26" spans="2:12" ht="18">
+      <c r="B26" s="228" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="142" t="s">
+        <v>334</v>
+      </c>
+      <c r="D26" s="143">
+        <v>8.6425494000000005E-2</v>
+      </c>
+      <c r="E26" s="144">
+        <v>7.9383789999999996E-2</v>
+      </c>
+      <c r="F26" s="151"/>
+    </row>
+    <row r="27" spans="2:12" ht="18">
+      <c r="B27" s="229"/>
+      <c r="C27" s="145" t="s">
+        <v>335</v>
+      </c>
+      <c r="D27" s="146">
+        <v>0.109670028</v>
+      </c>
+      <c r="E27" s="147">
+        <v>0.118666853</v>
+      </c>
+      <c r="F27" s="151"/>
+    </row>
+    <row r="28" spans="2:12" ht="18">
+      <c r="B28" s="229"/>
+      <c r="C28" s="145" t="s">
+        <v>336</v>
+      </c>
+      <c r="D28" s="146">
+        <v>0.16404260400000001</v>
+      </c>
+      <c r="E28" s="147">
+        <v>0.15010121400000001</v>
+      </c>
+      <c r="F28" s="151"/>
+    </row>
+    <row r="29" spans="2:12" ht="19" thickBot="1">
+      <c r="B29" s="230"/>
+      <c r="C29" s="148" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="149">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="E29" s="150">
+        <v>0.211236021</v>
+      </c>
+      <c r="F29" s="151"/>
+    </row>
+    <row r="30" spans="2:12" ht="18">
+      <c r="B30" s="241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="136" t="s">
+        <v>334</v>
+      </c>
+      <c r="D30" s="134">
+        <v>0.190903462</v>
+      </c>
+      <c r="E30" s="238" t="s">
+        <v>354</v>
+      </c>
+      <c r="F30" s="151"/>
+    </row>
+    <row r="31" spans="2:12" ht="18">
+      <c r="B31" s="226"/>
+      <c r="C31" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31" s="137">
+        <v>0.26741922000000001</v>
+      </c>
+      <c r="E31" s="239"/>
+      <c r="F31" s="151"/>
+    </row>
+    <row r="32" spans="2:12" ht="18">
+      <c r="B32" s="226"/>
+      <c r="C32" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D32" s="137">
+        <v>0.17281497700000001</v>
+      </c>
+      <c r="E32" s="239"/>
+      <c r="F32" s="151"/>
+    </row>
+    <row r="33" spans="2:7" ht="19" thickBot="1">
+      <c r="B33" s="227"/>
+      <c r="C33" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D33" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="E33" s="240"/>
+      <c r="F33" s="151"/>
+    </row>
+    <row r="34" spans="2:7" ht="18">
+      <c r="B34" s="151"/>
+      <c r="C34" s="151"/>
+      <c r="D34" s="151"/>
+      <c r="E34" s="151"/>
+      <c r="F34" s="151"/>
+    </row>
+    <row r="35" spans="2:7" ht="19" thickBot="1">
+      <c r="B35" s="151"/>
+      <c r="C35" s="151"/>
+      <c r="D35" s="151"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151"/>
+    </row>
+    <row r="36" spans="2:7" ht="18">
+      <c r="B36" s="222" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="224" t="s">
+        <v>333</v>
+      </c>
+      <c r="D36" s="236" t="s">
+        <v>351</v>
+      </c>
+      <c r="E36" s="246"/>
+      <c r="F36" s="246"/>
+      <c r="G36" s="237"/>
+    </row>
+    <row r="37" spans="2:7" ht="60" thickBot="1">
+      <c r="B37" s="223"/>
+      <c r="C37" s="225"/>
+      <c r="D37" s="130" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="130" t="s">
+        <v>352</v>
+      </c>
+      <c r="F37" s="152" t="s">
+        <v>353</v>
+      </c>
+      <c r="G37" s="152" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="18">
+      <c r="B38" s="226" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="133" t="s">
+        <v>334</v>
+      </c>
+      <c r="D38" s="134">
+        <v>8.2978075999999998E-2</v>
+      </c>
+      <c r="E38" s="135">
+        <v>9.2051521999999997E-2</v>
+      </c>
+      <c r="F38" s="135">
+        <v>0.73226722899999996</v>
+      </c>
+      <c r="G38" s="247" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="18">
+      <c r="B39" s="226"/>
+      <c r="C39" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D39" s="137">
+        <v>9.9679073000000007E-2</v>
+      </c>
+      <c r="E39" s="138">
+        <v>9.9730974E-2</v>
+      </c>
+      <c r="F39" s="138">
+        <v>0.49588315500000002</v>
+      </c>
+      <c r="G39" s="248"/>
+    </row>
+    <row r="40" spans="2:7" ht="18">
+      <c r="B40" s="226"/>
+      <c r="C40" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" s="137">
+        <v>2.9346153E-2</v>
+      </c>
+      <c r="E40" s="138">
+        <v>2.4776334000000001E-2</v>
+      </c>
+      <c r="F40" s="138">
+        <v>0.28808858799999998</v>
+      </c>
+      <c r="G40" s="248"/>
+    </row>
+    <row r="41" spans="2:7" ht="19" thickBot="1">
+      <c r="B41" s="227"/>
+      <c r="C41" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D41" s="140">
+        <v>0.13297837300000001</v>
+      </c>
+      <c r="E41" s="141">
+        <v>0.13796243799999999</v>
+      </c>
+      <c r="F41" s="141">
+        <v>0.93048497100000005</v>
+      </c>
+      <c r="G41" s="248"/>
+    </row>
+    <row r="42" spans="2:7" ht="18">
+      <c r="B42" s="228" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="142" t="s">
+        <v>334</v>
+      </c>
+      <c r="D42" s="143">
+        <v>8.6425494000000005E-2</v>
+      </c>
+      <c r="E42" s="144">
+        <v>0.16830964400000001</v>
+      </c>
+      <c r="F42" s="144">
+        <v>0.73510694799999998</v>
+      </c>
+      <c r="G42" s="248"/>
+    </row>
+    <row r="43" spans="2:7" ht="18">
+      <c r="B43" s="229"/>
+      <c r="C43" s="145" t="s">
+        <v>335</v>
+      </c>
+      <c r="D43" s="146">
+        <v>0.109670028</v>
+      </c>
+      <c r="E43" s="147">
+        <v>0.13232349900000001</v>
+      </c>
+      <c r="F43" s="147">
+        <v>0.375448901</v>
+      </c>
+      <c r="G43" s="248"/>
+    </row>
+    <row r="44" spans="2:7" ht="18">
+      <c r="B44" s="229"/>
+      <c r="C44" s="145" t="s">
+        <v>336</v>
+      </c>
+      <c r="D44" s="146">
+        <v>0.16404260400000001</v>
+      </c>
+      <c r="E44" s="147">
+        <v>0.14118240600000001</v>
+      </c>
+      <c r="F44" s="147">
+        <v>0.511421024</v>
+      </c>
+      <c r="G44" s="248"/>
+    </row>
+    <row r="45" spans="2:7" ht="19" thickBot="1">
+      <c r="B45" s="242"/>
+      <c r="C45" s="153" t="s">
+        <v>337</v>
+      </c>
+      <c r="D45" s="154">
+        <v>0.22100530099999999</v>
+      </c>
+      <c r="E45" s="155">
+        <v>0.25645743100000001</v>
+      </c>
+      <c r="F45" s="155">
+        <v>0.97103789200000001</v>
+      </c>
+      <c r="G45" s="248"/>
+    </row>
+    <row r="46" spans="2:7" ht="18">
+      <c r="B46" s="241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="156" t="s">
+        <v>334</v>
+      </c>
+      <c r="D46" s="157">
+        <v>0.190903462</v>
+      </c>
+      <c r="E46" s="157">
+        <v>0.181299869</v>
+      </c>
+      <c r="F46" s="243" t="s">
+        <v>354</v>
+      </c>
+      <c r="G46" s="248"/>
+    </row>
+    <row r="47" spans="2:7" ht="18">
+      <c r="B47" s="226"/>
+      <c r="C47" s="136" t="s">
+        <v>335</v>
+      </c>
+      <c r="D47" s="137">
+        <v>0.26741922000000001</v>
+      </c>
+      <c r="E47" s="137">
+        <v>0.208914723</v>
+      </c>
+      <c r="F47" s="244"/>
+      <c r="G47" s="248"/>
+    </row>
+    <row r="48" spans="2:7" ht="18">
+      <c r="B48" s="226"/>
+      <c r="C48" s="136" t="s">
+        <v>336</v>
+      </c>
+      <c r="D48" s="137">
+        <v>0.17281497700000001</v>
+      </c>
+      <c r="E48" s="137">
+        <v>0.14118196899999999</v>
+      </c>
+      <c r="F48" s="244"/>
+      <c r="G48" s="248"/>
+    </row>
+    <row r="49" spans="2:7" ht="19" thickBot="1">
+      <c r="B49" s="227"/>
+      <c r="C49" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D49" s="140">
+        <v>0.39427188000000002</v>
+      </c>
+      <c r="E49" s="158">
+        <v>0.310617427</v>
+      </c>
+      <c r="F49" s="245"/>
+      <c r="G49" s="249"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="G38:G49"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="F13:F16"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>